<commit_message>
feat: update language excel
</commit_message>
<xml_diff>
--- a/Excels/Language_多语言表.xlsx
+++ b/Excels/Language_多语言表.xlsx
@@ -1,31 +1,33 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27029"/>
-  <workbookPr defaultThemeVersion="166925"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="G:\MetaApp\Editor_Win64\MetaWorldSaved\Saved\MetaWorld\Project\Edit\DragonVerse\Excels\"/>
-    </mc:Choice>
-  </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{58AF11F7-531F-491E-BACE-A602E458BE62}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="xl" lastEdited="3" lowestEdited="5" rupBuild="9302"/>
+  <workbookPr/>
   <bookViews>
-    <workbookView xWindow="10380" yWindow="4020" windowWidth="28800" windowHeight="15345" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView windowWidth="24045" windowHeight="12375" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="0"/>
+  <calcPr calcId="191029"/>
   <extLst>
-    <ext xmlns:loext="http://schemas.libreoffice.org/" uri="{7626C862-2A13-11E5-B345-FEFF819CDC9F}">
-      <loext:extCalcPr stringRefSyntax="CalcA1ExcelA1"/>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
+        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
+        <xcalcf:feature name="microsoft.com:ARRAYTEXT_WF"/>
+      </xcalcf:calcFeatures>
     </ext>
   </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="340" uniqueCount="323">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="342" uniqueCount="325">
   <si>
     <t>int</t>
   </si>
@@ -182,7 +184,6 @@
         <sz val="10"/>
         <color rgb="FF000000"/>
         <rFont val="微软雅黑"/>
-        <family val="2"/>
         <charset val="134"/>
       </rPr>
       <t>ドラゴンバース</t>
@@ -192,7 +193,6 @@
         <sz val="10"/>
         <color rgb="FF000000"/>
         <rFont val="MS Gothic"/>
-        <family val="3"/>
         <charset val="128"/>
       </rPr>
       <t>・</t>
@@ -202,7 +202,6 @@
         <sz val="10"/>
         <color rgb="FF000000"/>
         <rFont val="微软雅黑"/>
-        <family val="2"/>
         <charset val="134"/>
       </rPr>
       <t>ネオってどんな世界?</t>
@@ -1024,12 +1023,24 @@
   <si>
     <t>过肩摔</t>
   </si>
+  <si>
+    <t>Dragontip_Content_0001</t>
+  </si>
+  <si>
+    <t>需要*元素龙才能解开该法阵！</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="5" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr9="http://schemas.microsoft.com/office/spreadsheetml/2016/revision9" mc:Ignorable="xr9">
+  <numFmts count="4">
+    <numFmt numFmtId="41" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
+    <numFmt numFmtId="42" formatCode="_ &quot;￥&quot;* #,##0_ ;_ &quot;￥&quot;* \-#,##0_ ;_ &quot;￥&quot;* &quot;-&quot;_ ;_ @_ "/>
+    <numFmt numFmtId="43" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
+    <numFmt numFmtId="44" formatCode="_ &quot;￥&quot;* #,##0.00_ ;_ &quot;￥&quot;* \-#,##0.00_ ;_ &quot;￥&quot;* &quot;-&quot;??_ ;_ @_ "/>
+  </numFmts>
+  <fonts count="24">
     <font>
       <sz val="10"/>
       <color rgb="FF000000"/>
@@ -1039,38 +1050,367 @@
     <font>
       <sz val="10"/>
       <color rgb="FF000000"/>
-      <name val="MS Gothic"/>
-      <family val="3"/>
-      <charset val="128"/>
-    </font>
-    <font>
-      <sz val="10"/>
-      <color rgb="FF000000"/>
       <name val="微软雅黑"/>
-      <family val="2"/>
       <charset val="134"/>
     </font>
     <font>
       <sz val="12"/>
       <name val="Calibri"/>
-      <family val="2"/>
+      <charset val="134"/>
     </font>
     <font>
-      <sz val="9"/>
-      <name val="宋体"/>
-      <family val="3"/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="等线"/>
       <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color rgb="FF0000FF"/>
+      <name val="等线"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color rgb="FF800080"/>
+      <name val="等线"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFF0000"/>
+      <name val="等线"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="18"/>
+      <color theme="3"/>
+      <name val="等线"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <i/>
+      <sz val="11"/>
+      <color rgb="FF7F7F7F"/>
+      <name val="等线"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="15"/>
+      <color theme="3"/>
+      <name val="等线"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="13"/>
+      <color theme="3"/>
+      <name val="等线"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="3"/>
+      <name val="等线"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF3F3F76"/>
+      <name val="等线"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FF3F3F3F"/>
+      <name val="等线"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FFFA7D00"/>
+      <name val="等线"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FFFFFFFF"/>
+      <name val="等线"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFA7D00"/>
+      <name val="等线"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="等线"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF006100"/>
+      <name val="等线"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C0006"/>
+      <name val="等线"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C6500"/>
+      <name val="等线"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="0"/>
+      <name val="等线"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="等线"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <color rgb="FF000000"/>
+      <name val="MS Gothic"/>
+      <charset val="128"/>
     </font>
   </fonts>
-  <fills count="2">
+  <fills count="33">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFFCC"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFCC99"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFF2F2F2"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFA5A5A5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFC6EFCE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFC7CE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFEB9C"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="1">
+  <borders count="9">
     <border>
       <left/>
       <right/>
@@ -1078,9 +1418,251 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color rgb="FFB2B2B2"/>
+      </left>
+      <right style="thin">
+        <color rgb="FFB2B2B2"/>
+      </right>
+      <top style="thin">
+        <color rgb="FFB2B2B2"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FFB2B2B2"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color theme="4"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color theme="4" tint="0.499984740745262"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF7F7F7F"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF7F7F7F"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF7F7F7F"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF7F7F7F"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF3F3F3F"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF3F3F3F"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF3F3F3F"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF3F3F3F"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="double">
+        <color rgb="FF3F3F3F"/>
+      </left>
+      <right style="double">
+        <color rgb="FF3F3F3F"/>
+      </right>
+      <top style="double">
+        <color rgb="FF3F3F3F"/>
+      </top>
+      <bottom style="double">
+        <color rgb="FF3F3F3F"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="double">
+        <color rgb="FFFF8001"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color theme="4"/>
+      </top>
+      <bottom style="double">
+        <color theme="4"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="49">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="43" fontId="3" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="44" fontId="3" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="9" fontId="3" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="41" fontId="3" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="42" fontId="3" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="1" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="3" borderId="4" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="4" borderId="5" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="4" borderId="4" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="5" borderId="6" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="7" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
   </cellStyleXfs>
   <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
@@ -1090,22 +1672,66 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="49">
     <cellStyle name="常规" xfId="0" builtinId="0"/>
+    <cellStyle name="千位分隔" xfId="1" builtinId="3"/>
+    <cellStyle name="货币" xfId="2" builtinId="4"/>
+    <cellStyle name="百分比" xfId="3" builtinId="5"/>
+    <cellStyle name="千位分隔[0]" xfId="4" builtinId="6"/>
+    <cellStyle name="货币[0]" xfId="5" builtinId="7"/>
+    <cellStyle name="超链接" xfId="6" builtinId="8"/>
+    <cellStyle name="已访问的超链接" xfId="7" builtinId="9"/>
+    <cellStyle name="注释" xfId="8" builtinId="10"/>
+    <cellStyle name="警告文本" xfId="9" builtinId="11"/>
+    <cellStyle name="标题" xfId="10" builtinId="15"/>
+    <cellStyle name="解释性文本" xfId="11" builtinId="53"/>
+    <cellStyle name="标题 1" xfId="12" builtinId="16"/>
+    <cellStyle name="标题 2" xfId="13" builtinId="17"/>
+    <cellStyle name="标题 3" xfId="14" builtinId="18"/>
+    <cellStyle name="标题 4" xfId="15" builtinId="19"/>
+    <cellStyle name="输入" xfId="16" builtinId="20"/>
+    <cellStyle name="输出" xfId="17" builtinId="21"/>
+    <cellStyle name="计算" xfId="18" builtinId="22"/>
+    <cellStyle name="检查单元格" xfId="19" builtinId="23"/>
+    <cellStyle name="链接单元格" xfId="20" builtinId="24"/>
+    <cellStyle name="汇总" xfId="21" builtinId="25"/>
+    <cellStyle name="好" xfId="22" builtinId="26"/>
+    <cellStyle name="差" xfId="23" builtinId="27"/>
+    <cellStyle name="适中" xfId="24" builtinId="28"/>
+    <cellStyle name="强调文字颜色 1" xfId="25" builtinId="29"/>
+    <cellStyle name="20% - 强调文字颜色 1" xfId="26" builtinId="30"/>
+    <cellStyle name="40% - 强调文字颜色 1" xfId="27" builtinId="31"/>
+    <cellStyle name="60% - 强调文字颜色 1" xfId="28" builtinId="32"/>
+    <cellStyle name="强调文字颜色 2" xfId="29" builtinId="33"/>
+    <cellStyle name="20% - 强调文字颜色 2" xfId="30" builtinId="34"/>
+    <cellStyle name="40% - 强调文字颜色 2" xfId="31" builtinId="35"/>
+    <cellStyle name="60% - 强调文字颜色 2" xfId="32" builtinId="36"/>
+    <cellStyle name="强调文字颜色 3" xfId="33" builtinId="37"/>
+    <cellStyle name="20% - 强调文字颜色 3" xfId="34" builtinId="38"/>
+    <cellStyle name="40% - 强调文字颜色 3" xfId="35" builtinId="39"/>
+    <cellStyle name="60% - 强调文字颜色 3" xfId="36" builtinId="40"/>
+    <cellStyle name="强调文字颜色 4" xfId="37" builtinId="41"/>
+    <cellStyle name="20% - 强调文字颜色 4" xfId="38" builtinId="42"/>
+    <cellStyle name="40% - 强调文字颜色 4" xfId="39" builtinId="43"/>
+    <cellStyle name="60% - 强调文字颜色 4" xfId="40" builtinId="44"/>
+    <cellStyle name="强调文字颜色 5" xfId="41" builtinId="45"/>
+    <cellStyle name="20% - 强调文字颜色 5" xfId="42" builtinId="46"/>
+    <cellStyle name="40% - 强调文字颜色 5" xfId="43" builtinId="47"/>
+    <cellStyle name="60% - 强调文字颜色 5" xfId="44" builtinId="48"/>
+    <cellStyle name="强调文字颜色 6" xfId="45" builtinId="49"/>
+    <cellStyle name="20% - 强调文字颜色 6" xfId="46" builtinId="50"/>
+    <cellStyle name="40% - 强调文字颜色 6" xfId="47" builtinId="51"/>
+    <cellStyle name="60% - 强调文字颜色 6" xfId="48" builtinId="52"/>
   </cellStyles>
-  <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
-    </ext>
-    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
-      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
     </ext>
   </extLst>
 </styleSheet>
@@ -1154,7 +1780,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
+        <a:latin typeface="Calibri Light"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="游ゴシック Light"/>
@@ -1187,26 +1813,9 @@
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
-        <a:font script="Armn" typeface="Arial"/>
-        <a:font script="Bugi" typeface="Leelawadee UI"/>
-        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
-        <a:font script="Java" typeface="Javanese Text"/>
-        <a:font script="Lisu" typeface="Segoe UI"/>
-        <a:font script="Mymr" typeface="Myanmar Text"/>
-        <a:font script="Nkoo" typeface="Ebrima"/>
-        <a:font script="Olck" typeface="Nirmala UI"/>
-        <a:font script="Osma" typeface="Ebrima"/>
-        <a:font script="Phag" typeface="Phagspa"/>
-        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
-        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
-        <a:font script="Syre" typeface="Estrangelo Edessa"/>
-        <a:font script="Sora" typeface="Nirmala UI"/>
-        <a:font script="Tale" typeface="Microsoft Tai Le"/>
-        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
-        <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
+        <a:latin typeface="Calibri"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="游ゴシック"/>
@@ -1239,23 +1848,6 @@
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
-        <a:font script="Armn" typeface="Arial"/>
-        <a:font script="Bugi" typeface="Leelawadee UI"/>
-        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
-        <a:font script="Java" typeface="Javanese Text"/>
-        <a:font script="Lisu" typeface="Segoe UI"/>
-        <a:font script="Mymr" typeface="Myanmar Text"/>
-        <a:font script="Nkoo" typeface="Ebrima"/>
-        <a:font script="Olck" typeface="Nirmala UI"/>
-        <a:font script="Osma" typeface="Ebrima"/>
-        <a:font script="Phag" typeface="Phagspa"/>
-        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
-        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
-        <a:font script="Syre" typeface="Estrangelo Edessa"/>
-        <a:font script="Sora" typeface="Nirmala UI"/>
-        <a:font script="Tale" typeface="Microsoft Tai Le"/>
-        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
-        <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -1397,24 +1989,19 @@
     </a:fmtScheme>
   </a:themeElements>
   <a:objectDefaults/>
-  <a:extraClrSchemeLst/>
-  <a:extLst>
-    <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
-    </a:ext>
-  </a:extLst>
 </a:theme>
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
+  <sheetPr/>
   <dimension ref="A1:F551"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="C17" sqref="C17"/>
+    <sheetView tabSelected="1" topLeftCell="A59" workbookViewId="0">
+      <selection activeCell="D84" sqref="D84"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.5" defaultRowHeight="16.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultColWidth="11.5" defaultRowHeight="16.5" outlineLevelCol="5"/>
   <cols>
     <col min="1" max="1" width="12.125" customWidth="1"/>
     <col min="2" max="2" width="34.625" customWidth="1"/>
@@ -1422,7 +2009,7 @@
     <col min="5" max="6" width="17.25" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" s="1" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="1" s="1" customFormat="1" spans="1:6">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -1442,7 +2029,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="2" spans="1:6" s="1" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="2" s="1" customFormat="1" spans="1:6">
       <c r="A2" s="1" t="s">
         <v>2</v>
       </c>
@@ -1462,7 +2049,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="3" spans="1:6" s="1" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="3" s="1" customFormat="1" spans="1:6">
       <c r="A3" s="1" t="s">
         <v>8</v>
       </c>
@@ -1482,7 +2069,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="4" spans="1:6" s="2" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="4" s="2" customFormat="1" spans="2:6">
       <c r="B4" s="2" t="s">
         <v>14</v>
       </c>
@@ -1499,7 +2086,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="5" spans="1:6" s="2" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="5" s="2" customFormat="1" spans="1:6">
       <c r="A5" s="2">
         <v>1</v>
       </c>
@@ -1519,7 +2106,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="6" spans="1:6" s="2" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="6" s="2" customFormat="1" spans="1:6">
       <c r="A6" s="2">
         <v>2</v>
       </c>
@@ -1539,7 +2126,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="7" spans="1:6" s="2" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="7" s="2" customFormat="1" spans="1:6">
       <c r="A7" s="2">
         <v>3</v>
       </c>
@@ -1559,7 +2146,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="8" spans="1:6" s="2" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="8" s="2" customFormat="1" spans="1:6">
       <c r="A8" s="2">
         <v>4</v>
       </c>
@@ -1579,7 +2166,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="9" spans="1:6" s="2" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="9" s="2" customFormat="1" spans="1:6">
       <c r="A9" s="2">
         <v>5</v>
       </c>
@@ -1599,7 +2186,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="10" spans="1:6" s="2" customFormat="1" ht="18.95" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="10" s="2" customFormat="1" ht="18.95" customHeight="1" spans="1:6">
       <c r="A10" s="2">
         <v>6</v>
       </c>
@@ -1619,7 +2206,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="11" spans="1:6" s="2" customFormat="1" ht="18.95" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="11" s="2" customFormat="1" ht="18.95" customHeight="1" spans="1:6">
       <c r="A11" s="2">
         <v>7</v>
       </c>
@@ -1639,7 +2226,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="12" spans="1:6" s="2" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="12" s="2" customFormat="1" spans="1:6">
       <c r="A12" s="2">
         <v>8</v>
       </c>
@@ -1659,7 +2246,7 @@
         <v>56</v>
       </c>
     </row>
-    <row r="13" spans="1:6" s="2" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="13" s="2" customFormat="1" spans="1:6">
       <c r="A13" s="2">
         <v>9</v>
       </c>
@@ -1679,7 +2266,7 @@
         <v>61</v>
       </c>
     </row>
-    <row r="14" spans="1:6" s="2" customFormat="1" ht="18.95" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="14" s="2" customFormat="1" ht="18.95" customHeight="1" spans="1:6">
       <c r="A14" s="2">
         <v>10</v>
       </c>
@@ -1699,7 +2286,7 @@
         <v>66</v>
       </c>
     </row>
-    <row r="15" spans="1:6" s="2" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="15" s="2" customFormat="1" spans="1:6">
       <c r="A15" s="2">
         <v>11</v>
       </c>
@@ -1719,7 +2306,7 @@
         <v>71</v>
       </c>
     </row>
-    <row r="16" spans="1:6" s="2" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="16" s="2" customFormat="1" spans="1:6">
       <c r="A16" s="2">
         <v>12</v>
       </c>
@@ -1739,7 +2326,7 @@
         <v>76</v>
       </c>
     </row>
-    <row r="17" spans="1:6" s="2" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="17" s="2" customFormat="1" spans="1:6">
       <c r="A17" s="2">
         <v>13</v>
       </c>
@@ -1759,7 +2346,7 @@
         <v>81</v>
       </c>
     </row>
-    <row r="18" spans="1:6" s="2" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="18" s="2" customFormat="1" spans="1:6">
       <c r="A18" s="2">
         <v>14</v>
       </c>
@@ -1779,7 +2366,7 @@
         <v>83</v>
       </c>
     </row>
-    <row r="19" spans="1:6" s="2" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="19" s="2" customFormat="1" spans="1:6">
       <c r="A19" s="2">
         <v>15</v>
       </c>
@@ -1799,7 +2386,7 @@
         <v>90</v>
       </c>
     </row>
-    <row r="20" spans="1:6" s="2" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="20" s="2" customFormat="1" spans="1:6">
       <c r="A20" s="2">
         <v>16</v>
       </c>
@@ -1819,7 +2406,7 @@
         <v>92</v>
       </c>
     </row>
-    <row r="21" spans="1:6" s="2" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="21" s="2" customFormat="1" spans="1:6">
       <c r="A21" s="2">
         <v>17</v>
       </c>
@@ -1839,7 +2426,7 @@
         <v>99</v>
       </c>
     </row>
-    <row r="22" spans="1:6" s="2" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="22" s="2" customFormat="1" spans="1:6">
       <c r="A22" s="2">
         <v>18</v>
       </c>
@@ -1859,7 +2446,7 @@
         <v>104</v>
       </c>
     </row>
-    <row r="23" spans="1:6" s="2" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="23" s="2" customFormat="1" spans="1:6">
       <c r="A23" s="2">
         <v>19</v>
       </c>
@@ -1879,7 +2466,7 @@
         <v>109</v>
       </c>
     </row>
-    <row r="24" spans="1:6" s="2" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="24" s="2" customFormat="1" spans="1:6">
       <c r="A24" s="2">
         <v>20</v>
       </c>
@@ -1899,7 +2486,7 @@
         <v>114</v>
       </c>
     </row>
-    <row r="25" spans="1:6" s="2" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="25" s="2" customFormat="1" spans="1:6">
       <c r="A25" s="2">
         <v>21</v>
       </c>
@@ -1919,7 +2506,7 @@
         <v>119</v>
       </c>
     </row>
-    <row r="26" spans="1:6" s="2" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="26" s="2" customFormat="1" spans="1:6">
       <c r="A26" s="2">
         <v>22</v>
       </c>
@@ -1939,7 +2526,7 @@
         <v>124</v>
       </c>
     </row>
-    <row r="27" spans="1:6" s="2" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="27" s="2" customFormat="1" spans="1:6">
       <c r="A27" s="2">
         <v>23</v>
       </c>
@@ -1959,7 +2546,7 @@
         <v>129</v>
       </c>
     </row>
-    <row r="28" spans="1:6" s="2" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="28" s="2" customFormat="1" spans="1:6">
       <c r="A28" s="2">
         <v>24</v>
       </c>
@@ -1979,7 +2566,7 @@
         <v>134</v>
       </c>
     </row>
-    <row r="29" spans="1:6" s="2" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="29" s="2" customFormat="1" spans="1:6">
       <c r="A29" s="2">
         <v>25</v>
       </c>
@@ -1999,7 +2586,7 @@
         <v>139</v>
       </c>
     </row>
-    <row r="30" spans="1:6" s="2" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="30" s="2" customFormat="1" spans="1:6">
       <c r="A30" s="2">
         <v>26</v>
       </c>
@@ -2019,7 +2606,7 @@
         <v>144</v>
       </c>
     </row>
-    <row r="31" spans="1:6" s="2" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="31" s="2" customFormat="1" spans="1:6">
       <c r="A31" s="2">
         <v>27</v>
       </c>
@@ -2039,7 +2626,7 @@
         <v>149</v>
       </c>
     </row>
-    <row r="32" spans="1:6" s="2" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="32" s="2" customFormat="1" spans="1:6">
       <c r="A32" s="2">
         <v>28</v>
       </c>
@@ -2059,7 +2646,7 @@
         <v>151</v>
       </c>
     </row>
-    <row r="33" spans="1:6" s="2" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="33" s="2" customFormat="1" spans="1:6">
       <c r="A33" s="2">
         <v>29</v>
       </c>
@@ -2079,7 +2666,7 @@
         <v>158</v>
       </c>
     </row>
-    <row r="34" spans="1:6" s="2" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="34" s="2" customFormat="1" spans="1:6">
       <c r="A34" s="2">
         <v>30</v>
       </c>
@@ -2099,7 +2686,7 @@
         <v>163</v>
       </c>
     </row>
-    <row r="35" spans="1:6" s="2" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="35" s="2" customFormat="1" spans="1:6">
       <c r="A35" s="2">
         <v>31</v>
       </c>
@@ -2119,7 +2706,7 @@
         <v>168</v>
       </c>
     </row>
-    <row r="36" spans="1:6" s="2" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="36" s="2" customFormat="1" spans="1:6">
       <c r="A36" s="2">
         <v>32</v>
       </c>
@@ -2139,7 +2726,7 @@
         <v>173</v>
       </c>
     </row>
-    <row r="37" spans="1:6" s="2" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="37" s="2" customFormat="1" spans="1:6">
       <c r="A37" s="2">
         <v>33</v>
       </c>
@@ -2159,7 +2746,7 @@
         <v>178</v>
       </c>
     </row>
-    <row r="38" spans="1:6" s="2" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="38" s="2" customFormat="1" spans="1:6">
       <c r="A38" s="2">
         <v>34</v>
       </c>
@@ -2179,7 +2766,7 @@
         <v>183</v>
       </c>
     </row>
-    <row r="39" spans="1:6" s="2" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="39" s="2" customFormat="1" spans="1:6">
       <c r="A39" s="2">
         <v>35</v>
       </c>
@@ -2199,7 +2786,7 @@
         <v>188</v>
       </c>
     </row>
-    <row r="40" spans="1:6" s="2" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="40" s="2" customFormat="1" spans="1:6">
       <c r="A40" s="2">
         <v>36</v>
       </c>
@@ -2219,7 +2806,7 @@
         <v>193</v>
       </c>
     </row>
-    <row r="41" spans="1:6" s="2" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="41" s="2" customFormat="1" spans="1:6">
       <c r="A41" s="2">
         <v>37</v>
       </c>
@@ -2239,7 +2826,7 @@
         <v>198</v>
       </c>
     </row>
-    <row r="42" spans="1:6" s="2" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="42" s="2" customFormat="1" spans="1:6">
       <c r="A42" s="2">
         <v>38</v>
       </c>
@@ -2259,7 +2846,7 @@
         <v>203</v>
       </c>
     </row>
-    <row r="43" spans="1:6" s="2" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="43" s="2" customFormat="1" spans="1:6">
       <c r="A43" s="2">
         <v>39</v>
       </c>
@@ -2279,7 +2866,7 @@
         <v>208</v>
       </c>
     </row>
-    <row r="44" spans="1:6" s="2" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="44" s="2" customFormat="1" spans="1:6">
       <c r="A44" s="2">
         <v>40</v>
       </c>
@@ -2299,7 +2886,7 @@
         <v>213</v>
       </c>
     </row>
-    <row r="45" spans="1:6" s="2" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="45" s="2" customFormat="1" spans="1:6">
       <c r="A45" s="2">
         <v>41</v>
       </c>
@@ -2319,7 +2906,7 @@
         <v>218</v>
       </c>
     </row>
-    <row r="46" spans="1:6" s="2" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="46" s="2" customFormat="1" spans="1:6">
       <c r="A46" s="2">
         <v>42</v>
       </c>
@@ -2339,7 +2926,7 @@
         <v>222</v>
       </c>
     </row>
-    <row r="47" spans="1:6" s="2" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="47" s="2" customFormat="1" spans="1:6">
       <c r="A47" s="2">
         <v>43</v>
       </c>
@@ -2359,7 +2946,7 @@
         <v>226</v>
       </c>
     </row>
-    <row r="48" spans="1:6" s="2" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="48" s="2" customFormat="1" spans="1:6">
       <c r="A48" s="2">
         <v>44</v>
       </c>
@@ -2379,7 +2966,7 @@
         <v>231</v>
       </c>
     </row>
-    <row r="49" spans="1:6" s="2" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="49" s="2" customFormat="1" spans="1:6">
       <c r="A49" s="2">
         <v>45</v>
       </c>
@@ -2399,7 +2986,7 @@
         <v>235</v>
       </c>
     </row>
-    <row r="50" spans="1:6" s="2" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="50" s="2" customFormat="1" spans="1:6">
       <c r="A50" s="2">
         <v>46</v>
       </c>
@@ -2419,8 +3006,8 @@
         <v>240</v>
       </c>
     </row>
-    <row r="51" spans="1:6" s="2" customFormat="1" x14ac:dyDescent="0.35"/>
-    <row r="52" spans="1:6" s="2" customFormat="1" ht="17.25" x14ac:dyDescent="0.35">
+    <row r="51" s="2" customFormat="1"/>
+    <row r="52" s="2" customFormat="1" spans="1:4">
       <c r="A52" s="3">
         <v>102129</v>
       </c>
@@ -2434,7 +3021,7 @@
         <v>243</v>
       </c>
     </row>
-    <row r="53" spans="1:6" s="2" customFormat="1" ht="17.25" x14ac:dyDescent="0.35">
+    <row r="53" s="2" customFormat="1" spans="1:4">
       <c r="A53" s="3">
         <v>102130</v>
       </c>
@@ -2448,7 +3035,7 @@
         <v>246</v>
       </c>
     </row>
-    <row r="54" spans="1:6" s="2" customFormat="1" ht="17.25" x14ac:dyDescent="0.35">
+    <row r="54" s="2" customFormat="1" spans="1:4">
       <c r="A54" s="3">
         <v>102131</v>
       </c>
@@ -2462,7 +3049,7 @@
         <v>249</v>
       </c>
     </row>
-    <row r="55" spans="1:6" s="2" customFormat="1" ht="17.25" x14ac:dyDescent="0.35">
+    <row r="55" s="2" customFormat="1" spans="1:4">
       <c r="A55" s="3">
         <v>102132</v>
       </c>
@@ -2476,7 +3063,7 @@
         <v>252</v>
       </c>
     </row>
-    <row r="56" spans="1:6" s="2" customFormat="1" ht="18.95" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="56" s="2" customFormat="1" ht="18.95" customHeight="1" spans="1:4">
       <c r="A56" s="3">
         <v>102133</v>
       </c>
@@ -2490,7 +3077,7 @@
         <v>255</v>
       </c>
     </row>
-    <row r="57" spans="1:6" s="2" customFormat="1" ht="18.95" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="57" s="2" customFormat="1" ht="18.95" customHeight="1" spans="1:4">
       <c r="A57" s="3">
         <v>102134</v>
       </c>
@@ -2504,7 +3091,7 @@
         <v>258</v>
       </c>
     </row>
-    <row r="58" spans="1:6" s="2" customFormat="1" ht="18.95" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="58" s="2" customFormat="1" ht="18.95" customHeight="1" spans="1:4">
       <c r="A58" s="3">
         <v>102135</v>
       </c>
@@ -2518,7 +3105,7 @@
         <v>261</v>
       </c>
     </row>
-    <row r="59" spans="1:6" s="2" customFormat="1" ht="18.95" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="59" s="2" customFormat="1" ht="18.95" customHeight="1" spans="1:4">
       <c r="A59" s="3">
         <v>102136</v>
       </c>
@@ -2532,7 +3119,7 @@
         <v>264</v>
       </c>
     </row>
-    <row r="60" spans="1:6" s="2" customFormat="1" ht="18.95" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="60" s="2" customFormat="1" ht="18.95" customHeight="1" spans="1:4">
       <c r="A60" s="3">
         <v>102137</v>
       </c>
@@ -2546,7 +3133,7 @@
         <v>267</v>
       </c>
     </row>
-    <row r="61" spans="1:6" s="2" customFormat="1" ht="18.95" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="61" s="2" customFormat="1" ht="18.95" customHeight="1" spans="1:4">
       <c r="A61" s="3">
         <v>102138</v>
       </c>
@@ -2560,7 +3147,7 @@
         <v>270</v>
       </c>
     </row>
-    <row r="62" spans="1:6" s="2" customFormat="1" ht="18.95" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="62" s="2" customFormat="1" ht="18.95" customHeight="1" spans="1:4">
       <c r="A62" s="3">
         <v>102139</v>
       </c>
@@ -2574,7 +3161,7 @@
         <v>273</v>
       </c>
     </row>
-    <row r="63" spans="1:6" s="2" customFormat="1" ht="17.25" x14ac:dyDescent="0.35">
+    <row r="63" s="2" customFormat="1" spans="1:4">
       <c r="A63" s="3">
         <v>102140</v>
       </c>
@@ -2588,7 +3175,7 @@
         <v>276</v>
       </c>
     </row>
-    <row r="64" spans="1:6" s="2" customFormat="1" ht="18.95" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="64" s="2" customFormat="1" ht="18.95" customHeight="1" spans="1:4">
       <c r="A64" s="3">
         <v>102141</v>
       </c>
@@ -2602,7 +3189,7 @@
         <v>279</v>
       </c>
     </row>
-    <row r="65" spans="1:4" s="2" customFormat="1" ht="18.95" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="65" s="2" customFormat="1" ht="18.95" customHeight="1" spans="1:4">
       <c r="A65" s="3">
         <v>102142</v>
       </c>
@@ -2616,7 +3203,7 @@
         <v>282</v>
       </c>
     </row>
-    <row r="66" spans="1:4" s="2" customFormat="1" ht="18.95" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="66" s="2" customFormat="1" ht="18.95" customHeight="1" spans="1:4">
       <c r="A66" s="3">
         <v>102143</v>
       </c>
@@ -2630,7 +3217,7 @@
         <v>284</v>
       </c>
     </row>
-    <row r="67" spans="1:4" s="2" customFormat="1" ht="18.95" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="67" s="2" customFormat="1" ht="18.95" customHeight="1" spans="1:4">
       <c r="A67" s="3">
         <v>102144</v>
       </c>
@@ -2644,7 +3231,7 @@
         <v>287</v>
       </c>
     </row>
-    <row r="68" spans="1:4" s="2" customFormat="1" ht="18.95" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="68" s="2" customFormat="1" ht="18.95" customHeight="1" spans="1:4">
       <c r="A68" s="3">
         <v>102145</v>
       </c>
@@ -2658,7 +3245,7 @@
         <v>290</v>
       </c>
     </row>
-    <row r="69" spans="1:4" s="2" customFormat="1" ht="18.95" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="69" s="2" customFormat="1" ht="18.95" customHeight="1" spans="1:4">
       <c r="A69" s="3">
         <v>102146</v>
       </c>
@@ -2672,7 +3259,7 @@
         <v>293</v>
       </c>
     </row>
-    <row r="70" spans="1:4" s="2" customFormat="1" ht="18.95" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="70" s="2" customFormat="1" ht="18.95" customHeight="1" spans="1:4">
       <c r="A70" s="3">
         <v>102147</v>
       </c>
@@ -2686,7 +3273,7 @@
         <v>296</v>
       </c>
     </row>
-    <row r="71" spans="1:4" s="2" customFormat="1" ht="18.95" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="71" s="2" customFormat="1" ht="18.95" customHeight="1" spans="1:4">
       <c r="A71" s="3">
         <v>102148</v>
       </c>
@@ -2700,7 +3287,7 @@
         <v>299</v>
       </c>
     </row>
-    <row r="72" spans="1:4" s="2" customFormat="1" ht="18.95" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="72" s="2" customFormat="1" ht="18.95" customHeight="1" spans="1:4">
       <c r="A72" s="3">
         <v>102149</v>
       </c>
@@ -2714,7 +3301,7 @@
         <v>302</v>
       </c>
     </row>
-    <row r="73" spans="1:4" s="2" customFormat="1" ht="18.95" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="73" s="2" customFormat="1" ht="18.95" customHeight="1" spans="1:4">
       <c r="A73" s="3">
         <v>102150</v>
       </c>
@@ -2728,7 +3315,7 @@
         <v>270</v>
       </c>
     </row>
-    <row r="74" spans="1:4" s="2" customFormat="1" ht="18.95" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="74" s="2" customFormat="1" ht="18.95" customHeight="1" spans="1:4">
       <c r="A74" s="3">
         <v>102151</v>
       </c>
@@ -2742,7 +3329,7 @@
         <v>306</v>
       </c>
     </row>
-    <row r="75" spans="1:4" s="2" customFormat="1" ht="18.95" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="75" s="2" customFormat="1" ht="18.95" customHeight="1" spans="1:4">
       <c r="A75" s="3">
         <v>102152</v>
       </c>
@@ -2756,7 +3343,7 @@
         <v>309</v>
       </c>
     </row>
-    <row r="76" spans="1:4" s="2" customFormat="1" ht="18.95" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="76" s="2" customFormat="1" ht="18.95" customHeight="1" spans="1:4">
       <c r="A76" s="3">
         <v>102153</v>
       </c>
@@ -2770,7 +3357,7 @@
         <v>312</v>
       </c>
     </row>
-    <row r="77" spans="1:4" s="2" customFormat="1" ht="18.95" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="77" s="2" customFormat="1" ht="18.95" customHeight="1" spans="1:4">
       <c r="A77" s="3">
         <v>102154</v>
       </c>
@@ -2784,7 +3371,7 @@
         <v>315</v>
       </c>
     </row>
-    <row r="78" spans="1:4" s="2" customFormat="1" ht="18.95" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="78" s="2" customFormat="1" ht="18.95" customHeight="1" spans="1:4">
       <c r="A78" s="3">
         <v>102155</v>
       </c>
@@ -2798,7 +3385,7 @@
         <v>318</v>
       </c>
     </row>
-    <row r="79" spans="1:4" s="2" customFormat="1" ht="18.95" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="79" s="2" customFormat="1" ht="18.95" customHeight="1" spans="1:4">
       <c r="A79" s="3">
         <v>102156</v>
       </c>
@@ -2812,7 +3399,7 @@
         <v>261</v>
       </c>
     </row>
-    <row r="80" spans="1:4" s="2" customFormat="1" ht="18.95" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="80" s="2" customFormat="1" ht="18.95" customHeight="1" spans="1:4">
       <c r="A80" s="3">
         <v>102157</v>
       </c>
@@ -2826,480 +3413,490 @@
         <v>322</v>
       </c>
     </row>
-    <row r="81" s="2" customFormat="1" ht="18.95" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="82" s="2" customFormat="1" ht="18.95" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="83" s="2" customFormat="1" ht="18.95" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="84" s="2" customFormat="1" ht="18.95" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="85" s="2" customFormat="1" ht="18.95" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="86" s="2" customFormat="1" ht="18.95" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="87" s="2" customFormat="1" ht="18.95" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="88" s="2" customFormat="1" ht="18.95" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="89" s="2" customFormat="1" ht="18.95" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="90" s="2" customFormat="1" ht="18.95" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="91" s="2" customFormat="1" ht="18.95" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="92" s="2" customFormat="1" ht="18.95" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="93" s="2" customFormat="1" ht="18.95" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="94" s="2" customFormat="1" ht="18.95" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="95" s="2" customFormat="1" ht="18.95" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="96" s="2" customFormat="1" x14ac:dyDescent="0.35"/>
-    <row r="97" s="2" customFormat="1" ht="18.95" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="98" s="2" customFormat="1" x14ac:dyDescent="0.35"/>
-    <row r="99" s="2" customFormat="1" ht="18.95" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="100" s="2" customFormat="1" ht="18.95" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="101" s="2" customFormat="1" ht="18.95" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="102" s="2" customFormat="1" ht="18.95" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="103" s="2" customFormat="1" ht="18.95" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="104" s="2" customFormat="1" ht="18.95" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="105" s="2" customFormat="1" ht="18.95" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="106" s="2" customFormat="1" ht="18.95" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="107" s="2" customFormat="1" ht="18.95" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="108" s="2" customFormat="1" ht="18.95" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="109" s="2" customFormat="1" ht="18.95" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="110" s="2" customFormat="1" ht="18.95" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="111" s="2" customFormat="1" x14ac:dyDescent="0.35"/>
-    <row r="112" s="2" customFormat="1" ht="18.95" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="113" s="2" customFormat="1" ht="18.95" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="114" s="2" customFormat="1" ht="18.95" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="115" s="2" customFormat="1" ht="18.95" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="116" s="2" customFormat="1" ht="18.95" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="117" s="2" customFormat="1" x14ac:dyDescent="0.35"/>
-    <row r="118" s="2" customFormat="1" ht="18.95" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="119" s="2" customFormat="1" ht="18.95" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="120" s="2" customFormat="1" ht="18.95" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="121" s="2" customFormat="1" ht="18.95" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="122" s="2" customFormat="1" ht="18.95" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="123" s="2" customFormat="1" ht="18.95" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="124" s="2" customFormat="1" ht="18.95" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="125" s="2" customFormat="1" ht="26.85" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="126" s="2" customFormat="1" ht="23.85" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="127" s="2" customFormat="1" ht="18.95" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="128" s="2" customFormat="1" ht="18.95" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="129" s="2" customFormat="1" ht="18.95" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="130" s="2" customFormat="1" ht="18.95" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="131" s="2" customFormat="1" ht="18.95" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="132" s="2" customFormat="1" ht="18.95" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="133" s="2" customFormat="1" ht="18.95" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="134" s="2" customFormat="1" x14ac:dyDescent="0.35"/>
-    <row r="135" s="2" customFormat="1" ht="18.95" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="136" s="2" customFormat="1" ht="18.95" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="137" s="2" customFormat="1" ht="18.95" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="138" s="2" customFormat="1" ht="18.95" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="139" s="2" customFormat="1" ht="18.95" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="140" s="2" customFormat="1" ht="18.95" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="141" s="2" customFormat="1" ht="18.95" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="142" s="2" customFormat="1" ht="18.95" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="143" s="2" customFormat="1" x14ac:dyDescent="0.35"/>
-    <row r="144" s="2" customFormat="1" x14ac:dyDescent="0.35"/>
-    <row r="145" s="2" customFormat="1" ht="18.95" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="146" s="2" customFormat="1" ht="18.95" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="147" s="2" customFormat="1" ht="18.95" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="148" s="2" customFormat="1" x14ac:dyDescent="0.35"/>
-    <row r="149" s="2" customFormat="1" ht="18.95" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="150" s="2" customFormat="1" ht="18.95" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="151" s="2" customFormat="1" ht="18.95" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="152" s="2" customFormat="1" ht="18.95" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="153" s="2" customFormat="1" ht="18.95" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="154" s="2" customFormat="1" ht="18.95" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="155" s="2" customFormat="1" ht="18.95" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="156" s="2" customFormat="1" ht="18.95" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="157" s="2" customFormat="1" ht="18.95" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="158" s="2" customFormat="1" ht="18.95" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="159" s="2" customFormat="1" ht="18.95" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="160" s="2" customFormat="1" ht="18.95" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="161" s="2" customFormat="1" ht="18.95" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="162" s="2" customFormat="1" ht="18.95" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="163" s="2" customFormat="1" ht="18.95" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="164" s="2" customFormat="1" ht="18.95" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="165" s="2" customFormat="1" ht="18.95" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="166" s="2" customFormat="1" ht="18.95" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="167" s="2" customFormat="1" ht="18.95" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="168" s="2" customFormat="1" ht="18.95" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="169" s="2" customFormat="1" ht="18.95" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="170" s="2" customFormat="1" ht="18.95" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="171" s="2" customFormat="1" ht="18.95" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="172" s="2" customFormat="1" ht="18.95" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="173" s="2" customFormat="1" ht="18.95" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="174" s="2" customFormat="1" ht="18.95" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="175" s="2" customFormat="1" ht="18.95" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="176" s="2" customFormat="1" ht="18.95" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="177" s="2" customFormat="1" ht="18.95" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="178" s="2" customFormat="1" ht="18.95" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="179" s="2" customFormat="1" ht="18.95" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="180" s="2" customFormat="1" ht="18.95" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="181" s="2" customFormat="1" ht="18.95" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="182" s="2" customFormat="1" ht="18.95" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="183" s="2" customFormat="1" ht="18.95" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="184" s="2" customFormat="1" x14ac:dyDescent="0.35"/>
-    <row r="185" s="2" customFormat="1" x14ac:dyDescent="0.35"/>
-    <row r="186" s="2" customFormat="1" x14ac:dyDescent="0.35"/>
-    <row r="187" s="2" customFormat="1" x14ac:dyDescent="0.35"/>
-    <row r="188" s="2" customFormat="1" x14ac:dyDescent="0.35"/>
-    <row r="189" s="2" customFormat="1" x14ac:dyDescent="0.35"/>
-    <row r="190" s="2" customFormat="1" x14ac:dyDescent="0.35"/>
-    <row r="191" s="2" customFormat="1" x14ac:dyDescent="0.35"/>
-    <row r="192" s="2" customFormat="1" x14ac:dyDescent="0.35"/>
-    <row r="193" s="2" customFormat="1" x14ac:dyDescent="0.35"/>
-    <row r="194" s="2" customFormat="1" x14ac:dyDescent="0.35"/>
-    <row r="195" s="2" customFormat="1" x14ac:dyDescent="0.35"/>
-    <row r="196" s="2" customFormat="1" x14ac:dyDescent="0.35"/>
-    <row r="197" s="2" customFormat="1" x14ac:dyDescent="0.35"/>
-    <row r="198" s="2" customFormat="1" x14ac:dyDescent="0.35"/>
-    <row r="199" s="2" customFormat="1" x14ac:dyDescent="0.35"/>
-    <row r="200" s="2" customFormat="1" x14ac:dyDescent="0.35"/>
-    <row r="201" s="2" customFormat="1" x14ac:dyDescent="0.35"/>
-    <row r="202" s="2" customFormat="1" x14ac:dyDescent="0.35"/>
-    <row r="203" s="2" customFormat="1" x14ac:dyDescent="0.35"/>
-    <row r="204" s="2" customFormat="1" x14ac:dyDescent="0.35"/>
-    <row r="205" s="2" customFormat="1" x14ac:dyDescent="0.35"/>
-    <row r="206" s="2" customFormat="1" x14ac:dyDescent="0.35"/>
-    <row r="207" s="2" customFormat="1" x14ac:dyDescent="0.35"/>
-    <row r="208" s="2" customFormat="1" x14ac:dyDescent="0.35"/>
-    <row r="209" s="2" customFormat="1" x14ac:dyDescent="0.35"/>
-    <row r="210" s="2" customFormat="1" x14ac:dyDescent="0.35"/>
-    <row r="211" s="2" customFormat="1" x14ac:dyDescent="0.35"/>
-    <row r="212" s="2" customFormat="1" x14ac:dyDescent="0.35"/>
-    <row r="213" s="2" customFormat="1" x14ac:dyDescent="0.35"/>
-    <row r="214" s="2" customFormat="1" x14ac:dyDescent="0.35"/>
-    <row r="215" s="2" customFormat="1" x14ac:dyDescent="0.35"/>
-    <row r="216" s="2" customFormat="1" x14ac:dyDescent="0.35"/>
-    <row r="217" s="2" customFormat="1" x14ac:dyDescent="0.35"/>
-    <row r="218" s="2" customFormat="1" x14ac:dyDescent="0.35"/>
-    <row r="219" s="2" customFormat="1" x14ac:dyDescent="0.35"/>
-    <row r="220" s="2" customFormat="1" x14ac:dyDescent="0.35"/>
-    <row r="221" s="2" customFormat="1" x14ac:dyDescent="0.35"/>
-    <row r="222" s="2" customFormat="1" x14ac:dyDescent="0.35"/>
-    <row r="223" s="2" customFormat="1" x14ac:dyDescent="0.35"/>
-    <row r="224" s="2" customFormat="1" x14ac:dyDescent="0.35"/>
-    <row r="225" s="2" customFormat="1" x14ac:dyDescent="0.35"/>
-    <row r="226" s="2" customFormat="1" x14ac:dyDescent="0.35"/>
-    <row r="227" s="2" customFormat="1" x14ac:dyDescent="0.35"/>
-    <row r="228" s="2" customFormat="1" x14ac:dyDescent="0.35"/>
-    <row r="229" s="2" customFormat="1" x14ac:dyDescent="0.35"/>
-    <row r="230" s="2" customFormat="1" x14ac:dyDescent="0.35"/>
-    <row r="231" s="2" customFormat="1" x14ac:dyDescent="0.35"/>
-    <row r="232" s="2" customFormat="1" x14ac:dyDescent="0.35"/>
-    <row r="233" s="2" customFormat="1" x14ac:dyDescent="0.35"/>
-    <row r="234" s="2" customFormat="1" x14ac:dyDescent="0.35"/>
-    <row r="235" s="2" customFormat="1" x14ac:dyDescent="0.35"/>
-    <row r="236" s="2" customFormat="1" x14ac:dyDescent="0.35"/>
-    <row r="237" s="2" customFormat="1" x14ac:dyDescent="0.35"/>
-    <row r="238" s="2" customFormat="1" x14ac:dyDescent="0.35"/>
-    <row r="239" s="2" customFormat="1" x14ac:dyDescent="0.35"/>
-    <row r="240" s="2" customFormat="1" x14ac:dyDescent="0.35"/>
-    <row r="241" s="2" customFormat="1" x14ac:dyDescent="0.35"/>
-    <row r="242" s="2" customFormat="1" x14ac:dyDescent="0.35"/>
-    <row r="243" s="2" customFormat="1" x14ac:dyDescent="0.35"/>
-    <row r="244" s="2" customFormat="1" x14ac:dyDescent="0.35"/>
-    <row r="245" s="2" customFormat="1" x14ac:dyDescent="0.35"/>
-    <row r="246" s="2" customFormat="1" x14ac:dyDescent="0.35"/>
-    <row r="247" s="2" customFormat="1" x14ac:dyDescent="0.35"/>
-    <row r="248" s="2" customFormat="1" x14ac:dyDescent="0.35"/>
-    <row r="249" s="2" customFormat="1" x14ac:dyDescent="0.35"/>
-    <row r="250" s="2" customFormat="1" x14ac:dyDescent="0.35"/>
-    <row r="251" s="2" customFormat="1" x14ac:dyDescent="0.35"/>
-    <row r="252" s="2" customFormat="1" x14ac:dyDescent="0.35"/>
-    <row r="253" s="2" customFormat="1" x14ac:dyDescent="0.35"/>
-    <row r="254" s="2" customFormat="1" x14ac:dyDescent="0.35"/>
-    <row r="255" s="2" customFormat="1" x14ac:dyDescent="0.35"/>
-    <row r="256" s="2" customFormat="1" x14ac:dyDescent="0.35"/>
-    <row r="257" s="2" customFormat="1" x14ac:dyDescent="0.35"/>
-    <row r="258" s="2" customFormat="1" x14ac:dyDescent="0.35"/>
-    <row r="259" s="2" customFormat="1" x14ac:dyDescent="0.35"/>
-    <row r="260" s="2" customFormat="1" x14ac:dyDescent="0.35"/>
-    <row r="261" s="2" customFormat="1" x14ac:dyDescent="0.35"/>
-    <row r="262" s="2" customFormat="1" x14ac:dyDescent="0.35"/>
-    <row r="263" s="2" customFormat="1" x14ac:dyDescent="0.35"/>
-    <row r="264" s="2" customFormat="1" x14ac:dyDescent="0.35"/>
-    <row r="265" s="2" customFormat="1" x14ac:dyDescent="0.35"/>
-    <row r="266" s="2" customFormat="1" x14ac:dyDescent="0.35"/>
-    <row r="267" s="2" customFormat="1" x14ac:dyDescent="0.35"/>
-    <row r="268" s="2" customFormat="1" x14ac:dyDescent="0.35"/>
-    <row r="269" s="2" customFormat="1" x14ac:dyDescent="0.35"/>
-    <row r="270" s="2" customFormat="1" x14ac:dyDescent="0.35"/>
-    <row r="271" s="2" customFormat="1" x14ac:dyDescent="0.35"/>
-    <row r="272" s="2" customFormat="1" x14ac:dyDescent="0.35"/>
-    <row r="273" s="2" customFormat="1" x14ac:dyDescent="0.35"/>
-    <row r="274" s="2" customFormat="1" x14ac:dyDescent="0.35"/>
-    <row r="275" s="2" customFormat="1" x14ac:dyDescent="0.35"/>
-    <row r="276" s="2" customFormat="1" x14ac:dyDescent="0.35"/>
-    <row r="277" s="2" customFormat="1" x14ac:dyDescent="0.35"/>
-    <row r="278" s="2" customFormat="1" x14ac:dyDescent="0.35"/>
-    <row r="279" s="2" customFormat="1" x14ac:dyDescent="0.35"/>
-    <row r="280" s="2" customFormat="1" x14ac:dyDescent="0.35"/>
-    <row r="281" s="2" customFormat="1" x14ac:dyDescent="0.35"/>
-    <row r="282" s="2" customFormat="1" x14ac:dyDescent="0.35"/>
-    <row r="283" s="2" customFormat="1" x14ac:dyDescent="0.35"/>
-    <row r="284" s="2" customFormat="1" x14ac:dyDescent="0.35"/>
-    <row r="285" s="2" customFormat="1" x14ac:dyDescent="0.35"/>
-    <row r="286" s="2" customFormat="1" x14ac:dyDescent="0.35"/>
-    <row r="287" s="2" customFormat="1" x14ac:dyDescent="0.35"/>
-    <row r="288" s="2" customFormat="1" x14ac:dyDescent="0.35"/>
-    <row r="289" s="2" customFormat="1" x14ac:dyDescent="0.35"/>
-    <row r="290" s="2" customFormat="1" x14ac:dyDescent="0.35"/>
-    <row r="291" s="2" customFormat="1" x14ac:dyDescent="0.35"/>
-    <row r="292" s="2" customFormat="1" x14ac:dyDescent="0.35"/>
-    <row r="293" s="2" customFormat="1" x14ac:dyDescent="0.35"/>
-    <row r="294" s="2" customFormat="1" x14ac:dyDescent="0.35"/>
-    <row r="295" s="2" customFormat="1" x14ac:dyDescent="0.35"/>
-    <row r="296" s="2" customFormat="1" x14ac:dyDescent="0.35"/>
-    <row r="297" s="2" customFormat="1" x14ac:dyDescent="0.35"/>
-    <row r="298" s="2" customFormat="1" x14ac:dyDescent="0.35"/>
-    <row r="299" s="2" customFormat="1" x14ac:dyDescent="0.35"/>
-    <row r="300" s="2" customFormat="1" x14ac:dyDescent="0.35"/>
-    <row r="301" s="2" customFormat="1" x14ac:dyDescent="0.35"/>
-    <row r="302" s="2" customFormat="1" x14ac:dyDescent="0.35"/>
-    <row r="303" s="2" customFormat="1" x14ac:dyDescent="0.35"/>
-    <row r="304" s="2" customFormat="1" x14ac:dyDescent="0.35"/>
-    <row r="305" s="2" customFormat="1" x14ac:dyDescent="0.35"/>
-    <row r="306" s="2" customFormat="1" x14ac:dyDescent="0.35"/>
-    <row r="307" s="2" customFormat="1" x14ac:dyDescent="0.35"/>
-    <row r="308" s="2" customFormat="1" x14ac:dyDescent="0.35"/>
-    <row r="309" s="2" customFormat="1" x14ac:dyDescent="0.35"/>
-    <row r="310" s="2" customFormat="1" x14ac:dyDescent="0.35"/>
-    <row r="311" s="2" customFormat="1" x14ac:dyDescent="0.35"/>
-    <row r="312" s="2" customFormat="1" x14ac:dyDescent="0.35"/>
-    <row r="313" s="2" customFormat="1" x14ac:dyDescent="0.35"/>
-    <row r="314" s="2" customFormat="1" x14ac:dyDescent="0.35"/>
-    <row r="315" s="2" customFormat="1" x14ac:dyDescent="0.35"/>
-    <row r="316" s="2" customFormat="1" x14ac:dyDescent="0.35"/>
-    <row r="317" s="2" customFormat="1" x14ac:dyDescent="0.35"/>
-    <row r="318" s="2" customFormat="1" x14ac:dyDescent="0.35"/>
-    <row r="319" s="2" customFormat="1" x14ac:dyDescent="0.35"/>
-    <row r="320" s="2" customFormat="1" x14ac:dyDescent="0.35"/>
-    <row r="321" s="2" customFormat="1" x14ac:dyDescent="0.35"/>
-    <row r="322" s="2" customFormat="1" x14ac:dyDescent="0.35"/>
-    <row r="323" s="2" customFormat="1" x14ac:dyDescent="0.35"/>
-    <row r="324" s="2" customFormat="1" x14ac:dyDescent="0.35"/>
-    <row r="325" s="2" customFormat="1" x14ac:dyDescent="0.35"/>
-    <row r="326" s="2" customFormat="1" x14ac:dyDescent="0.35"/>
-    <row r="327" s="2" customFormat="1" x14ac:dyDescent="0.35"/>
-    <row r="328" s="2" customFormat="1" x14ac:dyDescent="0.35"/>
-    <row r="329" s="2" customFormat="1" x14ac:dyDescent="0.35"/>
-    <row r="330" s="2" customFormat="1" x14ac:dyDescent="0.35"/>
-    <row r="331" s="2" customFormat="1" x14ac:dyDescent="0.35"/>
-    <row r="332" s="2" customFormat="1" x14ac:dyDescent="0.35"/>
-    <row r="333" s="2" customFormat="1" x14ac:dyDescent="0.35"/>
-    <row r="334" s="2" customFormat="1" x14ac:dyDescent="0.35"/>
-    <row r="335" s="2" customFormat="1" x14ac:dyDescent="0.35"/>
-    <row r="336" s="2" customFormat="1" x14ac:dyDescent="0.35"/>
-    <row r="337" s="2" customFormat="1" x14ac:dyDescent="0.35"/>
-    <row r="338" s="2" customFormat="1" x14ac:dyDescent="0.35"/>
-    <row r="339" s="2" customFormat="1" x14ac:dyDescent="0.35"/>
-    <row r="340" s="2" customFormat="1" x14ac:dyDescent="0.35"/>
-    <row r="341" s="2" customFormat="1" x14ac:dyDescent="0.35"/>
-    <row r="342" s="2" customFormat="1" x14ac:dyDescent="0.35"/>
-    <row r="343" s="2" customFormat="1" x14ac:dyDescent="0.35"/>
-    <row r="344" s="2" customFormat="1" x14ac:dyDescent="0.35"/>
-    <row r="345" s="2" customFormat="1" x14ac:dyDescent="0.35"/>
-    <row r="346" s="2" customFormat="1" x14ac:dyDescent="0.35"/>
-    <row r="347" s="2" customFormat="1" x14ac:dyDescent="0.35"/>
-    <row r="348" s="2" customFormat="1" x14ac:dyDescent="0.35"/>
-    <row r="349" s="2" customFormat="1" x14ac:dyDescent="0.35"/>
-    <row r="350" s="2" customFormat="1" x14ac:dyDescent="0.35"/>
-    <row r="351" s="2" customFormat="1" x14ac:dyDescent="0.35"/>
-    <row r="352" s="2" customFormat="1" x14ac:dyDescent="0.35"/>
-    <row r="353" s="2" customFormat="1" x14ac:dyDescent="0.35"/>
-    <row r="354" s="2" customFormat="1" x14ac:dyDescent="0.35"/>
-    <row r="355" s="2" customFormat="1" x14ac:dyDescent="0.35"/>
-    <row r="356" s="2" customFormat="1" x14ac:dyDescent="0.35"/>
-    <row r="357" s="2" customFormat="1" x14ac:dyDescent="0.35"/>
-    <row r="358" s="2" customFormat="1" x14ac:dyDescent="0.35"/>
-    <row r="359" s="2" customFormat="1" x14ac:dyDescent="0.35"/>
-    <row r="360" s="2" customFormat="1" x14ac:dyDescent="0.35"/>
-    <row r="361" s="2" customFormat="1" x14ac:dyDescent="0.35"/>
-    <row r="362" s="2" customFormat="1" x14ac:dyDescent="0.35"/>
-    <row r="363" s="2" customFormat="1" x14ac:dyDescent="0.35"/>
-    <row r="364" s="2" customFormat="1" x14ac:dyDescent="0.35"/>
-    <row r="365" s="2" customFormat="1" x14ac:dyDescent="0.35"/>
-    <row r="366" s="2" customFormat="1" x14ac:dyDescent="0.35"/>
-    <row r="367" s="2" customFormat="1" x14ac:dyDescent="0.35"/>
-    <row r="368" s="2" customFormat="1" x14ac:dyDescent="0.35"/>
-    <row r="369" s="2" customFormat="1" x14ac:dyDescent="0.35"/>
-    <row r="370" s="2" customFormat="1" x14ac:dyDescent="0.35"/>
-    <row r="371" s="2" customFormat="1" x14ac:dyDescent="0.35"/>
-    <row r="372" s="2" customFormat="1" x14ac:dyDescent="0.35"/>
-    <row r="373" s="2" customFormat="1" x14ac:dyDescent="0.35"/>
-    <row r="374" s="2" customFormat="1" x14ac:dyDescent="0.35"/>
-    <row r="375" s="2" customFormat="1" x14ac:dyDescent="0.35"/>
-    <row r="376" s="2" customFormat="1" x14ac:dyDescent="0.35"/>
-    <row r="377" s="2" customFormat="1" x14ac:dyDescent="0.35"/>
-    <row r="378" s="2" customFormat="1" x14ac:dyDescent="0.35"/>
-    <row r="379" s="2" customFormat="1" x14ac:dyDescent="0.35"/>
-    <row r="380" s="2" customFormat="1" x14ac:dyDescent="0.35"/>
-    <row r="381" s="2" customFormat="1" x14ac:dyDescent="0.35"/>
-    <row r="382" s="2" customFormat="1" x14ac:dyDescent="0.35"/>
-    <row r="383" s="2" customFormat="1" x14ac:dyDescent="0.35"/>
-    <row r="384" s="2" customFormat="1" x14ac:dyDescent="0.35"/>
-    <row r="385" s="2" customFormat="1" x14ac:dyDescent="0.35"/>
-    <row r="386" s="2" customFormat="1" x14ac:dyDescent="0.35"/>
-    <row r="387" s="2" customFormat="1" x14ac:dyDescent="0.35"/>
-    <row r="388" s="2" customFormat="1" x14ac:dyDescent="0.35"/>
-    <row r="389" s="2" customFormat="1" x14ac:dyDescent="0.35"/>
-    <row r="390" s="2" customFormat="1" x14ac:dyDescent="0.35"/>
-    <row r="391" s="2" customFormat="1" x14ac:dyDescent="0.35"/>
-    <row r="392" s="2" customFormat="1" x14ac:dyDescent="0.35"/>
-    <row r="393" s="2" customFormat="1" x14ac:dyDescent="0.35"/>
-    <row r="394" s="2" customFormat="1" x14ac:dyDescent="0.35"/>
-    <row r="395" s="2" customFormat="1" x14ac:dyDescent="0.35"/>
-    <row r="396" s="2" customFormat="1" x14ac:dyDescent="0.35"/>
-    <row r="397" s="2" customFormat="1" x14ac:dyDescent="0.35"/>
-    <row r="398" s="2" customFormat="1" x14ac:dyDescent="0.35"/>
-    <row r="399" s="2" customFormat="1" x14ac:dyDescent="0.35"/>
-    <row r="400" s="2" customFormat="1" x14ac:dyDescent="0.35"/>
-    <row r="401" s="2" customFormat="1" x14ac:dyDescent="0.35"/>
-    <row r="402" s="2" customFormat="1" x14ac:dyDescent="0.35"/>
-    <row r="403" s="2" customFormat="1" x14ac:dyDescent="0.35"/>
-    <row r="404" s="2" customFormat="1" x14ac:dyDescent="0.35"/>
-    <row r="405" s="2" customFormat="1" x14ac:dyDescent="0.35"/>
-    <row r="406" s="2" customFormat="1" x14ac:dyDescent="0.35"/>
-    <row r="407" s="2" customFormat="1" x14ac:dyDescent="0.35"/>
-    <row r="408" s="2" customFormat="1" x14ac:dyDescent="0.35"/>
-    <row r="409" s="2" customFormat="1" x14ac:dyDescent="0.35"/>
-    <row r="410" s="2" customFormat="1" x14ac:dyDescent="0.35"/>
-    <row r="411" s="2" customFormat="1" x14ac:dyDescent="0.35"/>
-    <row r="412" s="2" customFormat="1" x14ac:dyDescent="0.35"/>
-    <row r="413" s="2" customFormat="1" x14ac:dyDescent="0.35"/>
-    <row r="414" s="2" customFormat="1" x14ac:dyDescent="0.35"/>
-    <row r="415" s="2" customFormat="1" x14ac:dyDescent="0.35"/>
-    <row r="416" s="2" customFormat="1" x14ac:dyDescent="0.35"/>
-    <row r="417" s="2" customFormat="1" x14ac:dyDescent="0.35"/>
-    <row r="418" s="2" customFormat="1" x14ac:dyDescent="0.35"/>
-    <row r="419" s="2" customFormat="1" x14ac:dyDescent="0.35"/>
-    <row r="420" s="2" customFormat="1" x14ac:dyDescent="0.35"/>
-    <row r="421" s="2" customFormat="1" x14ac:dyDescent="0.35"/>
-    <row r="422" s="2" customFormat="1" x14ac:dyDescent="0.35"/>
-    <row r="423" s="2" customFormat="1" x14ac:dyDescent="0.35"/>
-    <row r="424" s="2" customFormat="1" x14ac:dyDescent="0.35"/>
-    <row r="425" s="2" customFormat="1" x14ac:dyDescent="0.35"/>
-    <row r="426" s="2" customFormat="1" x14ac:dyDescent="0.35"/>
-    <row r="427" s="2" customFormat="1" x14ac:dyDescent="0.35"/>
-    <row r="428" s="2" customFormat="1" x14ac:dyDescent="0.35"/>
-    <row r="429" s="2" customFormat="1" x14ac:dyDescent="0.35"/>
-    <row r="430" s="2" customFormat="1" x14ac:dyDescent="0.35"/>
-    <row r="431" s="2" customFormat="1" x14ac:dyDescent="0.35"/>
-    <row r="432" s="2" customFormat="1" x14ac:dyDescent="0.35"/>
-    <row r="433" s="2" customFormat="1" x14ac:dyDescent="0.35"/>
-    <row r="434" s="2" customFormat="1" x14ac:dyDescent="0.35"/>
-    <row r="435" s="2" customFormat="1" x14ac:dyDescent="0.35"/>
-    <row r="436" s="2" customFormat="1" x14ac:dyDescent="0.35"/>
-    <row r="437" s="2" customFormat="1" x14ac:dyDescent="0.35"/>
-    <row r="438" s="2" customFormat="1" x14ac:dyDescent="0.35"/>
-    <row r="439" s="2" customFormat="1" x14ac:dyDescent="0.35"/>
-    <row r="440" s="2" customFormat="1" x14ac:dyDescent="0.35"/>
-    <row r="441" s="2" customFormat="1" x14ac:dyDescent="0.35"/>
-    <row r="442" s="2" customFormat="1" x14ac:dyDescent="0.35"/>
-    <row r="443" s="2" customFormat="1" x14ac:dyDescent="0.35"/>
-    <row r="444" s="2" customFormat="1" x14ac:dyDescent="0.35"/>
-    <row r="445" s="2" customFormat="1" x14ac:dyDescent="0.35"/>
-    <row r="446" s="2" customFormat="1" x14ac:dyDescent="0.35"/>
-    <row r="447" s="2" customFormat="1" x14ac:dyDescent="0.35"/>
-    <row r="448" s="2" customFormat="1" x14ac:dyDescent="0.35"/>
-    <row r="449" s="2" customFormat="1" x14ac:dyDescent="0.35"/>
-    <row r="450" s="2" customFormat="1" x14ac:dyDescent="0.35"/>
-    <row r="451" s="2" customFormat="1" x14ac:dyDescent="0.35"/>
-    <row r="452" s="2" customFormat="1" ht="18.95" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="453" s="2" customFormat="1" ht="18.95" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="454" s="2" customFormat="1" ht="18.95" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="455" s="2" customFormat="1" ht="18.95" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="456" s="2" customFormat="1" ht="18.95" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="457" s="2" customFormat="1" ht="18.95" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="458" s="2" customFormat="1" x14ac:dyDescent="0.35"/>
-    <row r="459" s="2" customFormat="1" x14ac:dyDescent="0.35"/>
-    <row r="460" s="2" customFormat="1" x14ac:dyDescent="0.35"/>
-    <row r="461" s="2" customFormat="1" x14ac:dyDescent="0.35"/>
-    <row r="462" s="2" customFormat="1" x14ac:dyDescent="0.35"/>
-    <row r="463" s="2" customFormat="1" x14ac:dyDescent="0.35"/>
-    <row r="464" s="2" customFormat="1" x14ac:dyDescent="0.35"/>
-    <row r="465" s="2" customFormat="1" x14ac:dyDescent="0.35"/>
-    <row r="466" s="2" customFormat="1" x14ac:dyDescent="0.35"/>
-    <row r="467" s="2" customFormat="1" x14ac:dyDescent="0.35"/>
-    <row r="468" s="2" customFormat="1" x14ac:dyDescent="0.35"/>
-    <row r="469" s="2" customFormat="1" x14ac:dyDescent="0.35"/>
-    <row r="470" s="2" customFormat="1" x14ac:dyDescent="0.35"/>
-    <row r="471" s="2" customFormat="1" x14ac:dyDescent="0.35"/>
-    <row r="472" s="2" customFormat="1" x14ac:dyDescent="0.35"/>
-    <row r="473" s="2" customFormat="1" x14ac:dyDescent="0.35"/>
-    <row r="474" s="2" customFormat="1" x14ac:dyDescent="0.35"/>
-    <row r="475" s="2" customFormat="1" x14ac:dyDescent="0.35"/>
-    <row r="476" s="2" customFormat="1" x14ac:dyDescent="0.35"/>
-    <row r="477" s="2" customFormat="1" x14ac:dyDescent="0.35"/>
-    <row r="478" s="2" customFormat="1" x14ac:dyDescent="0.35"/>
-    <row r="479" s="2" customFormat="1" x14ac:dyDescent="0.35"/>
-    <row r="480" s="2" customFormat="1" x14ac:dyDescent="0.35"/>
-    <row r="481" s="2" customFormat="1" x14ac:dyDescent="0.35"/>
-    <row r="482" s="2" customFormat="1" x14ac:dyDescent="0.35"/>
-    <row r="483" s="2" customFormat="1" x14ac:dyDescent="0.35"/>
-    <row r="484" s="2" customFormat="1" x14ac:dyDescent="0.35"/>
-    <row r="485" s="2" customFormat="1" x14ac:dyDescent="0.35"/>
-    <row r="486" s="2" customFormat="1" x14ac:dyDescent="0.35"/>
-    <row r="487" s="2" customFormat="1" x14ac:dyDescent="0.35"/>
-    <row r="488" s="2" customFormat="1" x14ac:dyDescent="0.35"/>
-    <row r="489" s="2" customFormat="1" x14ac:dyDescent="0.35"/>
-    <row r="490" s="2" customFormat="1" x14ac:dyDescent="0.35"/>
-    <row r="491" s="2" customFormat="1" x14ac:dyDescent="0.35"/>
-    <row r="492" s="2" customFormat="1" x14ac:dyDescent="0.35"/>
-    <row r="493" s="2" customFormat="1" x14ac:dyDescent="0.35"/>
-    <row r="494" s="2" customFormat="1" x14ac:dyDescent="0.35"/>
-    <row r="495" s="2" customFormat="1" x14ac:dyDescent="0.35"/>
-    <row r="496" s="2" customFormat="1" x14ac:dyDescent="0.35"/>
-    <row r="497" s="2" customFormat="1" x14ac:dyDescent="0.35"/>
-    <row r="498" s="2" customFormat="1" x14ac:dyDescent="0.35"/>
-    <row r="499" s="2" customFormat="1" x14ac:dyDescent="0.35"/>
-    <row r="500" s="2" customFormat="1" x14ac:dyDescent="0.35"/>
-    <row r="501" s="2" customFormat="1" x14ac:dyDescent="0.35"/>
-    <row r="502" s="2" customFormat="1" x14ac:dyDescent="0.35"/>
-    <row r="503" s="2" customFormat="1" x14ac:dyDescent="0.35"/>
-    <row r="504" s="2" customFormat="1" x14ac:dyDescent="0.35"/>
-    <row r="505" s="2" customFormat="1" x14ac:dyDescent="0.35"/>
-    <row r="506" s="2" customFormat="1" x14ac:dyDescent="0.35"/>
-    <row r="507" s="2" customFormat="1" x14ac:dyDescent="0.35"/>
-    <row r="508" s="2" customFormat="1" x14ac:dyDescent="0.35"/>
-    <row r="509" s="2" customFormat="1" x14ac:dyDescent="0.35"/>
-    <row r="510" s="2" customFormat="1" x14ac:dyDescent="0.35"/>
-    <row r="511" s="2" customFormat="1" x14ac:dyDescent="0.35"/>
-    <row r="512" s="2" customFormat="1" x14ac:dyDescent="0.35"/>
-    <row r="513" s="2" customFormat="1" x14ac:dyDescent="0.35"/>
-    <row r="514" s="2" customFormat="1" x14ac:dyDescent="0.35"/>
-    <row r="515" s="2" customFormat="1" x14ac:dyDescent="0.35"/>
-    <row r="516" s="2" customFormat="1" x14ac:dyDescent="0.35"/>
-    <row r="517" s="2" customFormat="1" x14ac:dyDescent="0.35"/>
-    <row r="518" s="2" customFormat="1" x14ac:dyDescent="0.35"/>
-    <row r="519" s="2" customFormat="1" x14ac:dyDescent="0.35"/>
-    <row r="520" s="2" customFormat="1" x14ac:dyDescent="0.35"/>
-    <row r="521" s="2" customFormat="1" x14ac:dyDescent="0.35"/>
-    <row r="522" s="2" customFormat="1" x14ac:dyDescent="0.35"/>
-    <row r="523" s="2" customFormat="1" x14ac:dyDescent="0.35"/>
-    <row r="524" s="2" customFormat="1" x14ac:dyDescent="0.35"/>
-    <row r="525" s="2" customFormat="1" ht="18.600000000000001" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="526" s="2" customFormat="1" x14ac:dyDescent="0.35"/>
-    <row r="527" s="2" customFormat="1" x14ac:dyDescent="0.35"/>
-    <row r="528" s="2" customFormat="1" x14ac:dyDescent="0.35"/>
-    <row r="529" s="2" customFormat="1" x14ac:dyDescent="0.35"/>
-    <row r="530" s="2" customFormat="1" x14ac:dyDescent="0.35"/>
-    <row r="531" s="2" customFormat="1" x14ac:dyDescent="0.35"/>
-    <row r="532" s="2" customFormat="1" x14ac:dyDescent="0.35"/>
-    <row r="533" s="2" customFormat="1" x14ac:dyDescent="0.35"/>
-    <row r="534" s="2" customFormat="1" x14ac:dyDescent="0.35"/>
-    <row r="535" s="2" customFormat="1" x14ac:dyDescent="0.35"/>
-    <row r="536" s="2" customFormat="1" x14ac:dyDescent="0.35"/>
-    <row r="537" s="2" customFormat="1" x14ac:dyDescent="0.35"/>
-    <row r="538" s="2" customFormat="1" x14ac:dyDescent="0.35"/>
-    <row r="539" s="2" customFormat="1" x14ac:dyDescent="0.35"/>
-    <row r="540" s="2" customFormat="1" x14ac:dyDescent="0.35"/>
-    <row r="541" s="2" customFormat="1" x14ac:dyDescent="0.35"/>
-    <row r="542" s="2" customFormat="1" x14ac:dyDescent="0.35"/>
-    <row r="543" s="2" customFormat="1" x14ac:dyDescent="0.35"/>
-    <row r="544" s="2" customFormat="1" x14ac:dyDescent="0.35"/>
-    <row r="545" s="2" customFormat="1" x14ac:dyDescent="0.35"/>
-    <row r="546" s="2" customFormat="1" x14ac:dyDescent="0.35"/>
-    <row r="547" s="2" customFormat="1" x14ac:dyDescent="0.35"/>
-    <row r="548" s="2" customFormat="1" x14ac:dyDescent="0.35"/>
-    <row r="549" s="2" customFormat="1" x14ac:dyDescent="0.35"/>
-    <row r="550" s="2" customFormat="1" x14ac:dyDescent="0.35"/>
-    <row r="551" s="2" customFormat="1" x14ac:dyDescent="0.35"/>
+    <row r="81" s="2" customFormat="1" ht="18.95" customHeight="1" spans="1:4">
+      <c r="A81" s="2">
+        <v>102158</v>
+      </c>
+      <c r="B81" s="2" t="s">
+        <v>323</v>
+      </c>
+      <c r="D81" s="2" t="s">
+        <v>324</v>
+      </c>
+    </row>
+    <row r="82" s="2" customFormat="1" ht="18.95" customHeight="1"/>
+    <row r="83" s="2" customFormat="1" ht="18.95" customHeight="1"/>
+    <row r="84" s="2" customFormat="1" ht="18.95" customHeight="1"/>
+    <row r="85" s="2" customFormat="1" ht="18.95" customHeight="1"/>
+    <row r="86" s="2" customFormat="1" ht="18.95" customHeight="1"/>
+    <row r="87" s="2" customFormat="1" ht="18.95" customHeight="1"/>
+    <row r="88" s="2" customFormat="1" ht="18.95" customHeight="1"/>
+    <row r="89" s="2" customFormat="1" ht="18.95" customHeight="1"/>
+    <row r="90" s="2" customFormat="1" ht="18.95" customHeight="1"/>
+    <row r="91" s="2" customFormat="1" ht="18.95" customHeight="1"/>
+    <row r="92" s="2" customFormat="1" ht="18.95" customHeight="1"/>
+    <row r="93" s="2" customFormat="1" ht="18.95" customHeight="1"/>
+    <row r="94" s="2" customFormat="1" ht="18.95" customHeight="1"/>
+    <row r="95" s="2" customFormat="1" ht="18.95" customHeight="1"/>
+    <row r="96" s="2" customFormat="1"/>
+    <row r="97" s="2" customFormat="1" ht="18.95" customHeight="1"/>
+    <row r="98" s="2" customFormat="1"/>
+    <row r="99" s="2" customFormat="1" ht="18.95" customHeight="1"/>
+    <row r="100" s="2" customFormat="1" ht="18.95" customHeight="1"/>
+    <row r="101" s="2" customFormat="1" ht="18.95" customHeight="1"/>
+    <row r="102" s="2" customFormat="1" ht="18.95" customHeight="1"/>
+    <row r="103" s="2" customFormat="1" ht="18.95" customHeight="1"/>
+    <row r="104" s="2" customFormat="1" ht="18.95" customHeight="1"/>
+    <row r="105" s="2" customFormat="1" ht="18.95" customHeight="1"/>
+    <row r="106" s="2" customFormat="1" ht="18.95" customHeight="1"/>
+    <row r="107" s="2" customFormat="1" ht="18.95" customHeight="1"/>
+    <row r="108" s="2" customFormat="1" ht="18.95" customHeight="1"/>
+    <row r="109" s="2" customFormat="1" ht="18.95" customHeight="1"/>
+    <row r="110" s="2" customFormat="1" ht="18.95" customHeight="1"/>
+    <row r="111" s="2" customFormat="1"/>
+    <row r="112" s="2" customFormat="1" ht="18.95" customHeight="1"/>
+    <row r="113" s="2" customFormat="1" ht="18.95" customHeight="1"/>
+    <row r="114" s="2" customFormat="1" ht="18.95" customHeight="1"/>
+    <row r="115" s="2" customFormat="1" ht="18.95" customHeight="1"/>
+    <row r="116" s="2" customFormat="1" ht="18.95" customHeight="1"/>
+    <row r="117" s="2" customFormat="1"/>
+    <row r="118" s="2" customFormat="1" ht="18.95" customHeight="1"/>
+    <row r="119" s="2" customFormat="1" ht="18.95" customHeight="1"/>
+    <row r="120" s="2" customFormat="1" ht="18.95" customHeight="1"/>
+    <row r="121" s="2" customFormat="1" ht="18.95" customHeight="1"/>
+    <row r="122" s="2" customFormat="1" ht="18.95" customHeight="1"/>
+    <row r="123" s="2" customFormat="1" ht="18.95" customHeight="1"/>
+    <row r="124" s="2" customFormat="1" ht="18.95" customHeight="1"/>
+    <row r="125" s="2" customFormat="1" ht="26.85" customHeight="1"/>
+    <row r="126" s="2" customFormat="1" ht="23.85" customHeight="1"/>
+    <row r="127" s="2" customFormat="1" ht="18.95" customHeight="1"/>
+    <row r="128" s="2" customFormat="1" ht="18.95" customHeight="1"/>
+    <row r="129" s="2" customFormat="1" ht="18.95" customHeight="1"/>
+    <row r="130" s="2" customFormat="1" ht="18.95" customHeight="1"/>
+    <row r="131" s="2" customFormat="1" ht="18.95" customHeight="1"/>
+    <row r="132" s="2" customFormat="1" ht="18.95" customHeight="1"/>
+    <row r="133" s="2" customFormat="1" ht="18.95" customHeight="1"/>
+    <row r="134" s="2" customFormat="1"/>
+    <row r="135" s="2" customFormat="1" ht="18.95" customHeight="1"/>
+    <row r="136" s="2" customFormat="1" ht="18.95" customHeight="1"/>
+    <row r="137" s="2" customFormat="1" ht="18.95" customHeight="1"/>
+    <row r="138" s="2" customFormat="1" ht="18.95" customHeight="1"/>
+    <row r="139" s="2" customFormat="1" ht="18.95" customHeight="1"/>
+    <row r="140" s="2" customFormat="1" ht="18.95" customHeight="1"/>
+    <row r="141" s="2" customFormat="1" ht="18.95" customHeight="1"/>
+    <row r="142" s="2" customFormat="1" ht="18.95" customHeight="1"/>
+    <row r="143" s="2" customFormat="1"/>
+    <row r="144" s="2" customFormat="1"/>
+    <row r="145" s="2" customFormat="1" ht="18.95" customHeight="1"/>
+    <row r="146" s="2" customFormat="1" ht="18.95" customHeight="1"/>
+    <row r="147" s="2" customFormat="1" ht="18.95" customHeight="1"/>
+    <row r="148" s="2" customFormat="1"/>
+    <row r="149" s="2" customFormat="1" ht="18.95" customHeight="1"/>
+    <row r="150" s="2" customFormat="1" ht="18.95" customHeight="1"/>
+    <row r="151" s="2" customFormat="1" ht="18.95" customHeight="1"/>
+    <row r="152" s="2" customFormat="1" ht="18.95" customHeight="1"/>
+    <row r="153" s="2" customFormat="1" ht="18.95" customHeight="1"/>
+    <row r="154" s="2" customFormat="1" ht="18.95" customHeight="1"/>
+    <row r="155" s="2" customFormat="1" ht="18.95" customHeight="1"/>
+    <row r="156" s="2" customFormat="1" ht="18.95" customHeight="1"/>
+    <row r="157" s="2" customFormat="1" ht="18.95" customHeight="1"/>
+    <row r="158" s="2" customFormat="1" ht="18.95" customHeight="1"/>
+    <row r="159" s="2" customFormat="1" ht="18.95" customHeight="1"/>
+    <row r="160" s="2" customFormat="1" ht="18.95" customHeight="1"/>
+    <row r="161" s="2" customFormat="1" ht="18.95" customHeight="1"/>
+    <row r="162" s="2" customFormat="1" ht="18.95" customHeight="1"/>
+    <row r="163" s="2" customFormat="1" ht="18.95" customHeight="1"/>
+    <row r="164" s="2" customFormat="1" ht="18.95" customHeight="1"/>
+    <row r="165" s="2" customFormat="1" ht="18.95" customHeight="1"/>
+    <row r="166" s="2" customFormat="1" ht="18.95" customHeight="1"/>
+    <row r="167" s="2" customFormat="1" ht="18.95" customHeight="1"/>
+    <row r="168" s="2" customFormat="1" ht="18.95" customHeight="1"/>
+    <row r="169" s="2" customFormat="1" ht="18.95" customHeight="1"/>
+    <row r="170" s="2" customFormat="1" ht="18.95" customHeight="1"/>
+    <row r="171" s="2" customFormat="1" ht="18.95" customHeight="1"/>
+    <row r="172" s="2" customFormat="1" ht="18.95" customHeight="1"/>
+    <row r="173" s="2" customFormat="1" ht="18.95" customHeight="1"/>
+    <row r="174" s="2" customFormat="1" ht="18.95" customHeight="1"/>
+    <row r="175" s="2" customFormat="1" ht="18.95" customHeight="1"/>
+    <row r="176" s="2" customFormat="1" ht="18.95" customHeight="1"/>
+    <row r="177" s="2" customFormat="1" ht="18.95" customHeight="1"/>
+    <row r="178" s="2" customFormat="1" ht="18.95" customHeight="1"/>
+    <row r="179" s="2" customFormat="1" ht="18.95" customHeight="1"/>
+    <row r="180" s="2" customFormat="1" ht="18.95" customHeight="1"/>
+    <row r="181" s="2" customFormat="1" ht="18.95" customHeight="1"/>
+    <row r="182" s="2" customFormat="1" ht="18.95" customHeight="1"/>
+    <row r="183" s="2" customFormat="1" ht="18.95" customHeight="1"/>
+    <row r="184" s="2" customFormat="1"/>
+    <row r="185" s="2" customFormat="1"/>
+    <row r="186" s="2" customFormat="1"/>
+    <row r="187" s="2" customFormat="1"/>
+    <row r="188" s="2" customFormat="1"/>
+    <row r="189" s="2" customFormat="1"/>
+    <row r="190" s="2" customFormat="1"/>
+    <row r="191" s="2" customFormat="1"/>
+    <row r="192" s="2" customFormat="1"/>
+    <row r="193" s="2" customFormat="1"/>
+    <row r="194" s="2" customFormat="1"/>
+    <row r="195" s="2" customFormat="1"/>
+    <row r="196" s="2" customFormat="1"/>
+    <row r="197" s="2" customFormat="1"/>
+    <row r="198" s="2" customFormat="1"/>
+    <row r="199" s="2" customFormat="1"/>
+    <row r="200" s="2" customFormat="1"/>
+    <row r="201" s="2" customFormat="1"/>
+    <row r="202" s="2" customFormat="1"/>
+    <row r="203" s="2" customFormat="1"/>
+    <row r="204" s="2" customFormat="1"/>
+    <row r="205" s="2" customFormat="1"/>
+    <row r="206" s="2" customFormat="1"/>
+    <row r="207" s="2" customFormat="1"/>
+    <row r="208" s="2" customFormat="1"/>
+    <row r="209" s="2" customFormat="1"/>
+    <row r="210" s="2" customFormat="1"/>
+    <row r="211" s="2" customFormat="1"/>
+    <row r="212" s="2" customFormat="1"/>
+    <row r="213" s="2" customFormat="1"/>
+    <row r="214" s="2" customFormat="1"/>
+    <row r="215" s="2" customFormat="1"/>
+    <row r="216" s="2" customFormat="1"/>
+    <row r="217" s="2" customFormat="1"/>
+    <row r="218" s="2" customFormat="1"/>
+    <row r="219" s="2" customFormat="1"/>
+    <row r="220" s="2" customFormat="1"/>
+    <row r="221" s="2" customFormat="1"/>
+    <row r="222" s="2" customFormat="1"/>
+    <row r="223" s="2" customFormat="1"/>
+    <row r="224" s="2" customFormat="1"/>
+    <row r="225" s="2" customFormat="1"/>
+    <row r="226" s="2" customFormat="1"/>
+    <row r="227" s="2" customFormat="1"/>
+    <row r="228" s="2" customFormat="1"/>
+    <row r="229" s="2" customFormat="1"/>
+    <row r="230" s="2" customFormat="1"/>
+    <row r="231" s="2" customFormat="1"/>
+    <row r="232" s="2" customFormat="1"/>
+    <row r="233" s="2" customFormat="1"/>
+    <row r="234" s="2" customFormat="1"/>
+    <row r="235" s="2" customFormat="1"/>
+    <row r="236" s="2" customFormat="1"/>
+    <row r="237" s="2" customFormat="1"/>
+    <row r="238" s="2" customFormat="1"/>
+    <row r="239" s="2" customFormat="1"/>
+    <row r="240" s="2" customFormat="1"/>
+    <row r="241" s="2" customFormat="1"/>
+    <row r="242" s="2" customFormat="1"/>
+    <row r="243" s="2" customFormat="1"/>
+    <row r="244" s="2" customFormat="1"/>
+    <row r="245" s="2" customFormat="1"/>
+    <row r="246" s="2" customFormat="1"/>
+    <row r="247" s="2" customFormat="1"/>
+    <row r="248" s="2" customFormat="1"/>
+    <row r="249" s="2" customFormat="1"/>
+    <row r="250" s="2" customFormat="1"/>
+    <row r="251" s="2" customFormat="1"/>
+    <row r="252" s="2" customFormat="1"/>
+    <row r="253" s="2" customFormat="1"/>
+    <row r="254" s="2" customFormat="1"/>
+    <row r="255" s="2" customFormat="1"/>
+    <row r="256" s="2" customFormat="1"/>
+    <row r="257" s="2" customFormat="1"/>
+    <row r="258" s="2" customFormat="1"/>
+    <row r="259" s="2" customFormat="1"/>
+    <row r="260" s="2" customFormat="1"/>
+    <row r="261" s="2" customFormat="1"/>
+    <row r="262" s="2" customFormat="1"/>
+    <row r="263" s="2" customFormat="1"/>
+    <row r="264" s="2" customFormat="1"/>
+    <row r="265" s="2" customFormat="1"/>
+    <row r="266" s="2" customFormat="1"/>
+    <row r="267" s="2" customFormat="1"/>
+    <row r="268" s="2" customFormat="1"/>
+    <row r="269" s="2" customFormat="1"/>
+    <row r="270" s="2" customFormat="1"/>
+    <row r="271" s="2" customFormat="1"/>
+    <row r="272" s="2" customFormat="1"/>
+    <row r="273" s="2" customFormat="1"/>
+    <row r="274" s="2" customFormat="1"/>
+    <row r="275" s="2" customFormat="1"/>
+    <row r="276" s="2" customFormat="1"/>
+    <row r="277" s="2" customFormat="1"/>
+    <row r="278" s="2" customFormat="1"/>
+    <row r="279" s="2" customFormat="1"/>
+    <row r="280" s="2" customFormat="1"/>
+    <row r="281" s="2" customFormat="1"/>
+    <row r="282" s="2" customFormat="1"/>
+    <row r="283" s="2" customFormat="1"/>
+    <row r="284" s="2" customFormat="1"/>
+    <row r="285" s="2" customFormat="1"/>
+    <row r="286" s="2" customFormat="1"/>
+    <row r="287" s="2" customFormat="1"/>
+    <row r="288" s="2" customFormat="1"/>
+    <row r="289" s="2" customFormat="1"/>
+    <row r="290" s="2" customFormat="1"/>
+    <row r="291" s="2" customFormat="1"/>
+    <row r="292" s="2" customFormat="1"/>
+    <row r="293" s="2" customFormat="1"/>
+    <row r="294" s="2" customFormat="1"/>
+    <row r="295" s="2" customFormat="1"/>
+    <row r="296" s="2" customFormat="1"/>
+    <row r="297" s="2" customFormat="1"/>
+    <row r="298" s="2" customFormat="1"/>
+    <row r="299" s="2" customFormat="1"/>
+    <row r="300" s="2" customFormat="1"/>
+    <row r="301" s="2" customFormat="1"/>
+    <row r="302" s="2" customFormat="1"/>
+    <row r="303" s="2" customFormat="1"/>
+    <row r="304" s="2" customFormat="1"/>
+    <row r="305" s="2" customFormat="1"/>
+    <row r="306" s="2" customFormat="1"/>
+    <row r="307" s="2" customFormat="1"/>
+    <row r="308" s="2" customFormat="1"/>
+    <row r="309" s="2" customFormat="1"/>
+    <row r="310" s="2" customFormat="1"/>
+    <row r="311" s="2" customFormat="1"/>
+    <row r="312" s="2" customFormat="1"/>
+    <row r="313" s="2" customFormat="1"/>
+    <row r="314" s="2" customFormat="1"/>
+    <row r="315" s="2" customFormat="1"/>
+    <row r="316" s="2" customFormat="1"/>
+    <row r="317" s="2" customFormat="1"/>
+    <row r="318" s="2" customFormat="1"/>
+    <row r="319" s="2" customFormat="1"/>
+    <row r="320" s="2" customFormat="1"/>
+    <row r="321" s="2" customFormat="1"/>
+    <row r="322" s="2" customFormat="1"/>
+    <row r="323" s="2" customFormat="1"/>
+    <row r="324" s="2" customFormat="1"/>
+    <row r="325" s="2" customFormat="1"/>
+    <row r="326" s="2" customFormat="1"/>
+    <row r="327" s="2" customFormat="1"/>
+    <row r="328" s="2" customFormat="1"/>
+    <row r="329" s="2" customFormat="1"/>
+    <row r="330" s="2" customFormat="1"/>
+    <row r="331" s="2" customFormat="1"/>
+    <row r="332" s="2" customFormat="1"/>
+    <row r="333" s="2" customFormat="1"/>
+    <row r="334" s="2" customFormat="1"/>
+    <row r="335" s="2" customFormat="1"/>
+    <row r="336" s="2" customFormat="1"/>
+    <row r="337" s="2" customFormat="1"/>
+    <row r="338" s="2" customFormat="1"/>
+    <row r="339" s="2" customFormat="1"/>
+    <row r="340" s="2" customFormat="1"/>
+    <row r="341" s="2" customFormat="1"/>
+    <row r="342" s="2" customFormat="1"/>
+    <row r="343" s="2" customFormat="1"/>
+    <row r="344" s="2" customFormat="1"/>
+    <row r="345" s="2" customFormat="1"/>
+    <row r="346" s="2" customFormat="1"/>
+    <row r="347" s="2" customFormat="1"/>
+    <row r="348" s="2" customFormat="1"/>
+    <row r="349" s="2" customFormat="1"/>
+    <row r="350" s="2" customFormat="1"/>
+    <row r="351" s="2" customFormat="1"/>
+    <row r="352" s="2" customFormat="1"/>
+    <row r="353" s="2" customFormat="1"/>
+    <row r="354" s="2" customFormat="1"/>
+    <row r="355" s="2" customFormat="1"/>
+    <row r="356" s="2" customFormat="1"/>
+    <row r="357" s="2" customFormat="1"/>
+    <row r="358" s="2" customFormat="1"/>
+    <row r="359" s="2" customFormat="1"/>
+    <row r="360" s="2" customFormat="1"/>
+    <row r="361" s="2" customFormat="1"/>
+    <row r="362" s="2" customFormat="1"/>
+    <row r="363" s="2" customFormat="1"/>
+    <row r="364" s="2" customFormat="1"/>
+    <row r="365" s="2" customFormat="1"/>
+    <row r="366" s="2" customFormat="1"/>
+    <row r="367" s="2" customFormat="1"/>
+    <row r="368" s="2" customFormat="1"/>
+    <row r="369" s="2" customFormat="1"/>
+    <row r="370" s="2" customFormat="1"/>
+    <row r="371" s="2" customFormat="1"/>
+    <row r="372" s="2" customFormat="1"/>
+    <row r="373" s="2" customFormat="1"/>
+    <row r="374" s="2" customFormat="1"/>
+    <row r="375" s="2" customFormat="1"/>
+    <row r="376" s="2" customFormat="1"/>
+    <row r="377" s="2" customFormat="1"/>
+    <row r="378" s="2" customFormat="1"/>
+    <row r="379" s="2" customFormat="1"/>
+    <row r="380" s="2" customFormat="1"/>
+    <row r="381" s="2" customFormat="1"/>
+    <row r="382" s="2" customFormat="1"/>
+    <row r="383" s="2" customFormat="1"/>
+    <row r="384" s="2" customFormat="1"/>
+    <row r="385" s="2" customFormat="1"/>
+    <row r="386" s="2" customFormat="1"/>
+    <row r="387" s="2" customFormat="1"/>
+    <row r="388" s="2" customFormat="1"/>
+    <row r="389" s="2" customFormat="1"/>
+    <row r="390" s="2" customFormat="1"/>
+    <row r="391" s="2" customFormat="1"/>
+    <row r="392" s="2" customFormat="1"/>
+    <row r="393" s="2" customFormat="1"/>
+    <row r="394" s="2" customFormat="1"/>
+    <row r="395" s="2" customFormat="1"/>
+    <row r="396" s="2" customFormat="1"/>
+    <row r="397" s="2" customFormat="1"/>
+    <row r="398" s="2" customFormat="1"/>
+    <row r="399" s="2" customFormat="1"/>
+    <row r="400" s="2" customFormat="1"/>
+    <row r="401" s="2" customFormat="1"/>
+    <row r="402" s="2" customFormat="1"/>
+    <row r="403" s="2" customFormat="1"/>
+    <row r="404" s="2" customFormat="1"/>
+    <row r="405" s="2" customFormat="1"/>
+    <row r="406" s="2" customFormat="1"/>
+    <row r="407" s="2" customFormat="1"/>
+    <row r="408" s="2" customFormat="1"/>
+    <row r="409" s="2" customFormat="1"/>
+    <row r="410" s="2" customFormat="1"/>
+    <row r="411" s="2" customFormat="1"/>
+    <row r="412" s="2" customFormat="1"/>
+    <row r="413" s="2" customFormat="1"/>
+    <row r="414" s="2" customFormat="1"/>
+    <row r="415" s="2" customFormat="1"/>
+    <row r="416" s="2" customFormat="1"/>
+    <row r="417" s="2" customFormat="1"/>
+    <row r="418" s="2" customFormat="1"/>
+    <row r="419" s="2" customFormat="1"/>
+    <row r="420" s="2" customFormat="1"/>
+    <row r="421" s="2" customFormat="1"/>
+    <row r="422" s="2" customFormat="1"/>
+    <row r="423" s="2" customFormat="1"/>
+    <row r="424" s="2" customFormat="1"/>
+    <row r="425" s="2" customFormat="1"/>
+    <row r="426" s="2" customFormat="1"/>
+    <row r="427" s="2" customFormat="1"/>
+    <row r="428" s="2" customFormat="1"/>
+    <row r="429" s="2" customFormat="1"/>
+    <row r="430" s="2" customFormat="1"/>
+    <row r="431" s="2" customFormat="1"/>
+    <row r="432" s="2" customFormat="1"/>
+    <row r="433" s="2" customFormat="1"/>
+    <row r="434" s="2" customFormat="1"/>
+    <row r="435" s="2" customFormat="1"/>
+    <row r="436" s="2" customFormat="1"/>
+    <row r="437" s="2" customFormat="1"/>
+    <row r="438" s="2" customFormat="1"/>
+    <row r="439" s="2" customFormat="1"/>
+    <row r="440" s="2" customFormat="1"/>
+    <row r="441" s="2" customFormat="1"/>
+    <row r="442" s="2" customFormat="1"/>
+    <row r="443" s="2" customFormat="1"/>
+    <row r="444" s="2" customFormat="1"/>
+    <row r="445" s="2" customFormat="1"/>
+    <row r="446" s="2" customFormat="1"/>
+    <row r="447" s="2" customFormat="1"/>
+    <row r="448" s="2" customFormat="1"/>
+    <row r="449" s="2" customFormat="1"/>
+    <row r="450" s="2" customFormat="1"/>
+    <row r="451" s="2" customFormat="1"/>
+    <row r="452" s="2" customFormat="1" ht="18.95" customHeight="1"/>
+    <row r="453" s="2" customFormat="1" ht="18.95" customHeight="1"/>
+    <row r="454" s="2" customFormat="1" ht="18.95" customHeight="1"/>
+    <row r="455" s="2" customFormat="1" ht="18.95" customHeight="1"/>
+    <row r="456" s="2" customFormat="1" ht="18.95" customHeight="1"/>
+    <row r="457" s="2" customFormat="1" ht="18.95" customHeight="1"/>
+    <row r="458" s="2" customFormat="1"/>
+    <row r="459" s="2" customFormat="1"/>
+    <row r="460" s="2" customFormat="1"/>
+    <row r="461" s="2" customFormat="1"/>
+    <row r="462" s="2" customFormat="1"/>
+    <row r="463" s="2" customFormat="1"/>
+    <row r="464" s="2" customFormat="1"/>
+    <row r="465" s="2" customFormat="1"/>
+    <row r="466" s="2" customFormat="1"/>
+    <row r="467" s="2" customFormat="1"/>
+    <row r="468" s="2" customFormat="1"/>
+    <row r="469" s="2" customFormat="1"/>
+    <row r="470" s="2" customFormat="1"/>
+    <row r="471" s="2" customFormat="1"/>
+    <row r="472" s="2" customFormat="1"/>
+    <row r="473" s="2" customFormat="1"/>
+    <row r="474" s="2" customFormat="1"/>
+    <row r="475" s="2" customFormat="1"/>
+    <row r="476" s="2" customFormat="1"/>
+    <row r="477" s="2" customFormat="1"/>
+    <row r="478" s="2" customFormat="1"/>
+    <row r="479" s="2" customFormat="1"/>
+    <row r="480" s="2" customFormat="1"/>
+    <row r="481" s="2" customFormat="1"/>
+    <row r="482" s="2" customFormat="1"/>
+    <row r="483" s="2" customFormat="1"/>
+    <row r="484" s="2" customFormat="1"/>
+    <row r="485" s="2" customFormat="1"/>
+    <row r="486" s="2" customFormat="1"/>
+    <row r="487" s="2" customFormat="1"/>
+    <row r="488" s="2" customFormat="1"/>
+    <row r="489" s="2" customFormat="1"/>
+    <row r="490" s="2" customFormat="1"/>
+    <row r="491" s="2" customFormat="1"/>
+    <row r="492" s="2" customFormat="1"/>
+    <row r="493" s="2" customFormat="1"/>
+    <row r="494" s="2" customFormat="1"/>
+    <row r="495" s="2" customFormat="1"/>
+    <row r="496" s="2" customFormat="1"/>
+    <row r="497" s="2" customFormat="1"/>
+    <row r="498" s="2" customFormat="1"/>
+    <row r="499" s="2" customFormat="1"/>
+    <row r="500" s="2" customFormat="1"/>
+    <row r="501" s="2" customFormat="1"/>
+    <row r="502" s="2" customFormat="1"/>
+    <row r="503" s="2" customFormat="1"/>
+    <row r="504" s="2" customFormat="1"/>
+    <row r="505" s="2" customFormat="1"/>
+    <row r="506" s="2" customFormat="1"/>
+    <row r="507" s="2" customFormat="1"/>
+    <row r="508" s="2" customFormat="1"/>
+    <row r="509" s="2" customFormat="1"/>
+    <row r="510" s="2" customFormat="1"/>
+    <row r="511" s="2" customFormat="1"/>
+    <row r="512" s="2" customFormat="1"/>
+    <row r="513" s="2" customFormat="1"/>
+    <row r="514" s="2" customFormat="1"/>
+    <row r="515" s="2" customFormat="1"/>
+    <row r="516" s="2" customFormat="1"/>
+    <row r="517" s="2" customFormat="1"/>
+    <row r="518" s="2" customFormat="1"/>
+    <row r="519" s="2" customFormat="1"/>
+    <row r="520" s="2" customFormat="1"/>
+    <row r="521" s="2" customFormat="1"/>
+    <row r="522" s="2" customFormat="1"/>
+    <row r="523" s="2" customFormat="1"/>
+    <row r="524" s="2" customFormat="1"/>
+    <row r="525" s="2" customFormat="1" ht="18.6" customHeight="1"/>
+    <row r="526" s="2" customFormat="1"/>
+    <row r="527" s="2" customFormat="1"/>
+    <row r="528" s="2" customFormat="1"/>
+    <row r="529" s="2" customFormat="1"/>
+    <row r="530" s="2" customFormat="1"/>
+    <row r="531" s="2" customFormat="1"/>
+    <row r="532" s="2" customFormat="1"/>
+    <row r="533" s="2" customFormat="1"/>
+    <row r="534" s="2" customFormat="1"/>
+    <row r="535" s="2" customFormat="1"/>
+    <row r="536" s="2" customFormat="1"/>
+    <row r="537" s="2" customFormat="1"/>
+    <row r="538" s="2" customFormat="1"/>
+    <row r="539" s="2" customFormat="1"/>
+    <row r="540" s="2" customFormat="1"/>
+    <row r="541" s="2" customFormat="1"/>
+    <row r="542" s="2" customFormat="1"/>
+    <row r="543" s="2" customFormat="1"/>
+    <row r="544" s="2" customFormat="1"/>
+    <row r="545" s="2" customFormat="1"/>
+    <row r="546" s="2" customFormat="1"/>
+    <row r="547" s="2" customFormat="1"/>
+    <row r="548" s="2" customFormat="1"/>
+    <row r="549" s="2" customFormat="1"/>
+    <row r="550" s="2" customFormat="1"/>
+    <row r="551" s="2" customFormat="1"/>
   </sheetData>
-  <phoneticPr fontId="4" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511811023622047" footer="0.511811023622047"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="300"/>
+  <headerFooter/>
 </worksheet>
 </file>
</xml_diff>